<commit_message>
Added txt file containing questions
</commit_message>
<xml_diff>
--- a/Gantt Chart.xlsx
+++ b/Gantt Chart.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC89658C-A5E7-4C3D-ADBA-C71CA3640167}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E607CE41-D0B6-4ACE-8DA0-4B20EB511218}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
   <si>
     <t>Project Start:</t>
   </si>
@@ -230,6 +230,9 @@
   </si>
   <si>
     <t>Actual Time (Late)</t>
+  </si>
+  <si>
+    <t>Questions</t>
   </si>
 </sst>
 </file>
@@ -900,7 +903,68 @@
     <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkUp">
+          <fgColor rgb="FF80BA4C"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1088,15 +1152,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="17"/>
-      <tableStyleElement type="headerRow" dxfId="16"/>
-      <tableStyleElement type="totalRow" dxfId="15"/>
-      <tableStyleElement type="firstColumn" dxfId="14"/>
-      <tableStyleElement type="lastColumn" dxfId="13"/>
-      <tableStyleElement type="firstRowStripe" dxfId="12"/>
-      <tableStyleElement type="secondRowStripe" dxfId="11"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="10"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="9"/>
+      <tableStyleElement type="wholeTable" dxfId="23"/>
+      <tableStyleElement type="headerRow" dxfId="22"/>
+      <tableStyleElement type="totalRow" dxfId="21"/>
+      <tableStyleElement type="firstColumn" dxfId="20"/>
+      <tableStyleElement type="lastColumn" dxfId="19"/>
+      <tableStyleElement type="firstRowStripe" dxfId="18"/>
+      <tableStyleElement type="secondRowStripe" dxfId="17"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="16"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="15"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1512,11 +1576,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BQ22"/>
+  <dimension ref="A1:BQ23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W11" sqref="W11"/>
+      <selection pane="bottomLeft" activeCell="AC19" sqref="AC19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2387,7 +2451,7 @@
       </c>
       <c r="G9" s="62"/>
       <c r="H9" s="16">
-        <f t="shared" ref="H9:H19" si="10">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H9:H20" si="10">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v>60</v>
       </c>
       <c r="I9" s="26"/>
@@ -2550,12 +2614,12 @@
         <v>0</v>
       </c>
       <c r="E11" s="52">
-        <f>F10</f>
-        <v>44003</v>
+        <f>F10+1</f>
+        <v>44004</v>
       </c>
       <c r="F11" s="52">
         <f>E11+1</f>
-        <v>44004</v>
+        <v>44005</v>
       </c>
       <c r="G11" s="62"/>
       <c r="H11" s="16">
@@ -2634,7 +2698,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="52">
-        <f>F11+1</f>
+        <f>E11+1</f>
         <v>44005</v>
       </c>
       <c r="F12" s="52">
@@ -2784,26 +2848,26 @@
       <c r="BQ13" s="73"/>
     </row>
     <row r="14" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="40"/>
+      <c r="A14" s="39"/>
       <c r="B14" s="57" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C14" s="50"/>
       <c r="D14" s="25">
         <v>0</v>
       </c>
       <c r="E14" s="55">
-        <f>F12-2</f>
-        <v>44010</v>
+        <f>E15</f>
+        <v>44009</v>
       </c>
       <c r="F14" s="55">
-        <f>E14+21</f>
-        <v>44031</v>
+        <f>E14+2</f>
+        <v>44011</v>
       </c>
       <c r="G14" s="63"/>
       <c r="H14" s="16">
         <f t="shared" si="10"/>
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="I14" s="68"/>
       <c r="J14" s="68"/>
@@ -2821,7 +2885,7 @@
       <c r="V14" s="68"/>
       <c r="W14" s="68"/>
       <c r="X14" s="68"/>
-      <c r="Y14" s="68"/>
+      <c r="Y14" s="69"/>
       <c r="Z14" s="68"/>
       <c r="AA14" s="68"/>
       <c r="AB14" s="68"/>
@@ -2868,24 +2932,26 @@
       <c r="BQ14" s="75"/>
     </row>
     <row r="15" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="39"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="57" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C15" s="50"/>
-      <c r="D15" s="25"/>
+      <c r="D15" s="25">
+        <v>0</v>
+      </c>
       <c r="E15" s="55">
-        <f>F14-7</f>
-        <v>44024</v>
+        <f>F12-3</f>
+        <v>44009</v>
       </c>
       <c r="F15" s="55">
-        <f>E15+7</f>
-        <v>44031</v>
+        <f>E15+21</f>
+        <v>44030</v>
       </c>
       <c r="G15" s="63"/>
       <c r="H15" s="16">
         <f t="shared" si="10"/>
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="I15" s="68"/>
       <c r="J15" s="68"/>
@@ -2903,7 +2969,7 @@
       <c r="V15" s="68"/>
       <c r="W15" s="68"/>
       <c r="X15" s="68"/>
-      <c r="Y15" s="69"/>
+      <c r="Y15" s="68"/>
       <c r="Z15" s="68"/>
       <c r="AA15" s="68"/>
       <c r="AB15" s="68"/>
@@ -2952,24 +3018,24 @@
     <row r="16" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="39"/>
       <c r="B16" s="57" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C16" s="50"/>
       <c r="D16" s="25">
         <v>0</v>
       </c>
       <c r="E16" s="55">
-        <f>F14-7</f>
-        <v>44024</v>
+        <f>F15-7</f>
+        <v>44023</v>
       </c>
       <c r="F16" s="55">
-        <f>E16+10</f>
-        <v>44034</v>
+        <f>E16+7</f>
+        <v>44030</v>
       </c>
       <c r="G16" s="63"/>
       <c r="H16" s="16">
         <f t="shared" si="10"/>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I16" s="68"/>
       <c r="J16" s="68"/>
@@ -2983,11 +3049,11 @@
       <c r="R16" s="68"/>
       <c r="S16" s="68"/>
       <c r="T16" s="68"/>
-      <c r="U16" s="69"/>
-      <c r="V16" s="69"/>
+      <c r="U16" s="68"/>
+      <c r="V16" s="68"/>
       <c r="W16" s="68"/>
       <c r="X16" s="68"/>
-      <c r="Y16" s="68"/>
+      <c r="Y16" s="69"/>
       <c r="Z16" s="68"/>
       <c r="AA16" s="68"/>
       <c r="AB16" s="68"/>
@@ -3036,17 +3102,19 @@
     <row r="17" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="39"/>
       <c r="B17" s="57" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C17" s="50"/>
-      <c r="D17" s="25"/>
+      <c r="D17" s="25">
+        <v>0</v>
+      </c>
       <c r="E17" s="55">
-        <f>F16</f>
-        <v>44034</v>
+        <f>F15-7</f>
+        <v>44023</v>
       </c>
       <c r="F17" s="55">
         <f>E17+10</f>
-        <v>44044</v>
+        <v>44033</v>
       </c>
       <c r="G17" s="63"/>
       <c r="H17" s="16">
@@ -3065,8 +3133,8 @@
       <c r="R17" s="68"/>
       <c r="S17" s="68"/>
       <c r="T17" s="68"/>
-      <c r="U17" s="68"/>
-      <c r="V17" s="68"/>
+      <c r="U17" s="69"/>
+      <c r="V17" s="69"/>
       <c r="W17" s="68"/>
       <c r="X17" s="68"/>
       <c r="Y17" s="68"/>
@@ -3118,22 +3186,24 @@
     <row r="18" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="39"/>
       <c r="B18" s="57" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C18" s="50"/>
-      <c r="D18" s="25"/>
+      <c r="D18" s="25">
+        <v>0</v>
+      </c>
       <c r="E18" s="55">
-        <f>E19</f>
-        <v>44039</v>
+        <f>F17-3</f>
+        <v>44030</v>
       </c>
       <c r="F18" s="55">
-        <f>E18+9</f>
-        <v>44048</v>
+        <f>E18+10</f>
+        <v>44040</v>
       </c>
       <c r="G18" s="63"/>
       <c r="H18" s="16">
         <f t="shared" si="10"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I18" s="68"/>
       <c r="J18" s="68"/>
@@ -3200,22 +3270,24 @@
     <row r="19" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="39"/>
       <c r="B19" s="57" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C19" s="50"/>
-      <c r="D19" s="25"/>
+      <c r="D19" s="25">
+        <v>0</v>
+      </c>
       <c r="E19" s="55">
-        <f>F17-5</f>
-        <v>44039</v>
+        <f>F17</f>
+        <v>44033</v>
       </c>
       <c r="F19" s="55">
-        <f>E19+12</f>
-        <v>44051</v>
+        <f>E19+9</f>
+        <v>44042</v>
       </c>
       <c r="G19" s="63"/>
       <c r="H19" s="16">
         <f t="shared" si="10"/>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I19" s="68"/>
       <c r="J19" s="68"/>
@@ -3279,15 +3351,99 @@
       <c r="BP19" s="68"/>
       <c r="BQ19" s="75"/>
     </row>
-    <row r="20" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G20" s="6"/>
+    <row r="20" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="39"/>
+      <c r="B20" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="50"/>
+      <c r="D20" s="25">
+        <v>0</v>
+      </c>
+      <c r="E20" s="55">
+        <f>F19-5</f>
+        <v>44037</v>
+      </c>
+      <c r="F20" s="55">
+        <f>E20+12</f>
+        <v>44049</v>
+      </c>
+      <c r="G20" s="63"/>
+      <c r="H20" s="16">
+        <f t="shared" si="10"/>
+        <v>13</v>
+      </c>
+      <c r="I20" s="68"/>
+      <c r="J20" s="68"/>
+      <c r="K20" s="68"/>
+      <c r="L20" s="68"/>
+      <c r="M20" s="68"/>
+      <c r="N20" s="68"/>
+      <c r="O20" s="68"/>
+      <c r="P20" s="68"/>
+      <c r="Q20" s="68"/>
+      <c r="R20" s="68"/>
+      <c r="S20" s="68"/>
+      <c r="T20" s="68"/>
+      <c r="U20" s="68"/>
+      <c r="V20" s="68"/>
+      <c r="W20" s="68"/>
+      <c r="X20" s="68"/>
+      <c r="Y20" s="68"/>
+      <c r="Z20" s="68"/>
+      <c r="AA20" s="68"/>
+      <c r="AB20" s="68"/>
+      <c r="AC20" s="68"/>
+      <c r="AD20" s="68"/>
+      <c r="AE20" s="68"/>
+      <c r="AF20" s="68"/>
+      <c r="AG20" s="68"/>
+      <c r="AH20" s="68"/>
+      <c r="AI20" s="68"/>
+      <c r="AJ20" s="68"/>
+      <c r="AK20" s="68"/>
+      <c r="AL20" s="68"/>
+      <c r="AM20" s="68"/>
+      <c r="AN20" s="68"/>
+      <c r="AO20" s="68"/>
+      <c r="AP20" s="68"/>
+      <c r="AQ20" s="68"/>
+      <c r="AR20" s="68"/>
+      <c r="AS20" s="68"/>
+      <c r="AT20" s="68"/>
+      <c r="AU20" s="68"/>
+      <c r="AV20" s="68"/>
+      <c r="AW20" s="68"/>
+      <c r="AX20" s="68"/>
+      <c r="AY20" s="68"/>
+      <c r="AZ20" s="68"/>
+      <c r="BA20" s="68"/>
+      <c r="BB20" s="68"/>
+      <c r="BC20" s="68"/>
+      <c r="BD20" s="68"/>
+      <c r="BE20" s="68"/>
+      <c r="BF20" s="68"/>
+      <c r="BG20" s="68"/>
+      <c r="BH20" s="68"/>
+      <c r="BI20" s="68"/>
+      <c r="BJ20" s="68"/>
+      <c r="BK20" s="68"/>
+      <c r="BL20" s="68"/>
+      <c r="BM20" s="68"/>
+      <c r="BN20" s="68"/>
+      <c r="BO20" s="68"/>
+      <c r="BP20" s="68"/>
+      <c r="BQ20" s="75"/>
     </row>
     <row r="21" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="14"/>
-      <c r="F21" s="41"/>
+      <c r="G21" s="6"/>
     </row>
     <row r="22" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="15"/>
+      <c r="C22" s="14"/>
+      <c r="F22" s="41"/>
+    </row>
+    <row r="23" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -3304,8 +3460,8 @@
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
   </mergeCells>
-  <conditionalFormatting sqref="AF8:AF9 BH8:BH9 D7:D19">
-    <cfRule type="dataBar" priority="24">
+  <conditionalFormatting sqref="AF8:AF9 BH8:BH9 D7:D20">
+    <cfRule type="dataBar" priority="31">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3318,21 +3474,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BP7 I9:BP12 I19:BL19 I14:BP18 BM18:BP19">
-    <cfRule type="expression" dxfId="8" priority="43">
+  <conditionalFormatting sqref="I5:BP7 I9:BP12 I20:BL20 BM19:BP20 I15:BP19">
+    <cfRule type="expression" dxfId="14" priority="50">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BP7 I9:BP12 I19:BL19 I14:BP18 BM18:BP19">
-    <cfRule type="expression" dxfId="7" priority="37">
+  <conditionalFormatting sqref="I7:BP7 I9:BP12 I20:BL20 BM19:BP20 I15:BP19">
+    <cfRule type="expression" dxfId="13" priority="44">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="45" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D18">
-    <cfRule type="dataBar" priority="4">
+  <conditionalFormatting sqref="D19">
+    <cfRule type="dataBar" priority="11">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -3345,29 +3501,69 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I18:BL18">
-    <cfRule type="expression" dxfId="5" priority="7">
+  <conditionalFormatting sqref="I19:BL19">
+    <cfRule type="expression" dxfId="11" priority="14">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I18:BL18">
-    <cfRule type="expression" dxfId="4" priority="5">
+  <conditionalFormatting sqref="I19:BL19">
+    <cfRule type="expression" dxfId="10" priority="12">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="13" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BQ5:BQ7 BQ9:BQ12 BQ14:BQ19">
-    <cfRule type="expression" dxfId="2" priority="45">
+  <conditionalFormatting sqref="BQ5:BQ7 BQ9:BQ12 BQ15:BQ20">
+    <cfRule type="expression" dxfId="8" priority="52">
       <formula>AND(TODAY()&gt;=BQ$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BQ7 BQ9:BQ12 BQ14:BQ19">
-    <cfRule type="expression" dxfId="1" priority="48">
+  <conditionalFormatting sqref="BQ7 BQ9:BQ12 BQ15:BQ20">
+    <cfRule type="expression" dxfId="7" priority="55">
       <formula>AND(task_start&lt;=BQ$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BQ$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="56" stopIfTrue="1">
+      <formula>AND(task_end&gt;=BQ$5,task_start&lt;#REF!)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{788803AA-61D0-401D-A7E2-8CCEAE2E2732}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14:BP14">
+    <cfRule type="expression" dxfId="5" priority="4">
+      <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14:BP14">
+    <cfRule type="expression" dxfId="4" priority="2">
+      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
+      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BQ14">
+    <cfRule type="expression" dxfId="2" priority="5">
+      <formula>AND(TODAY()&gt;=BQ$5,TODAY()&lt;#REF!)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BQ14">
+    <cfRule type="expression" dxfId="1" priority="6">
+      <formula>AND(task_start&lt;=BQ$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BQ$5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="7" stopIfTrue="1">
       <formula>AND(task_end&gt;=BQ$5,task_start&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3402,7 +3598,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>AF8:AF9 BH8:BH9 D7:D19</xm:sqref>
+          <xm:sqref>AF8:AF9 BH8:BH9 D7:D20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{B11F1B6D-5EC8-4017-96F0-3B2262CAA45A}">
@@ -3417,7 +3613,22 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D18</xm:sqref>
+          <xm:sqref>D19</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{788803AA-61D0-401D-A7E2-8CCEAE2E2732}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D14</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3429,7 +3640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Updated Gantt chart to display elapsed time for Parts 1 and 2.
</commit_message>
<xml_diff>
--- a/Gantt Chart.xlsx
+++ b/Gantt Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7493C1-20F7-4B1B-AEAF-68CE8B7AB95F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA71ADEC-D87C-4578-9709-1E4F2C30BAD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,9 +12,9 @@
     <sheet name="About" sheetId="12" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Display_Week">ProjectSchedule!$F$5</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">ProjectSchedule!$5:$7</definedName>
-    <definedName name="Project_Start">ProjectSchedule!$F$4</definedName>
+    <definedName name="Display_Week">ProjectSchedule!$F$6</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">ProjectSchedule!$6:$8</definedName>
+    <definedName name="Project_Start">ProjectSchedule!$F$5</definedName>
     <definedName name="task_end" localSheetId="0">ProjectSchedule!$F1</definedName>
     <definedName name="task_progress" localSheetId="0">ProjectSchedule!$D1</definedName>
     <definedName name="task_start" localSheetId="0">ProjectSchedule!$E1</definedName>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
   <si>
     <t>Project Start:</t>
   </si>
@@ -237,19 +237,26 @@
   <si>
     <t>Research and define the problem + IPO</t>
   </si>
+  <si>
+    <t>Percentage Elapsed:</t>
+  </si>
+  <si>
+    <t>Ahead/Behind:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="166" formatCode="ddd\,\ m/d/yyyy"/>
     <numFmt numFmtId="167" formatCode="mmm\ d\,\ yyyy"/>
     <numFmt numFmtId="168" formatCode="d"/>
     <numFmt numFmtId="169" formatCode="d/mm/yy;@"/>
-    <numFmt numFmtId="173" formatCode="ddd\ d/m/yy"/>
+    <numFmt numFmtId="170" formatCode="ddd\ d/m/yy"/>
+    <numFmt numFmtId="171" formatCode="\+#,##0.00%;[Red]\-#,##0.00%"/>
   </numFmts>
   <fonts count="28" x14ac:knownFonts="1">
     <font>
@@ -1310,7 +1317,7 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1439,30 +1446,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="7" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="4" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1475,12 +1461,6 @@
     <xf numFmtId="9" fontId="4" fillId="3" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1511,9 +1491,6 @@
     <xf numFmtId="9" fontId="4" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1544,9 +1521,6 @@
     <xf numFmtId="169" fontId="7" fillId="2" borderId="25" xfId="10" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="169" fontId="7" fillId="2" borderId="26" xfId="10" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1571,7 +1545,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1581,12 +1555,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="169" fontId="7" fillId="3" borderId="32" xfId="10" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1629,40 +1597,68 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="168" fontId="9" fillId="4" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="26" fillId="11" borderId="0" xfId="13" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="55" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="53" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="56" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="52" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="54" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="52" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="53" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="54" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="55" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="56" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="9" fillId="4" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="26" fillId="11" borderId="0" xfId="13" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="48" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -1693,11 +1689,35 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="59" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="60" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="27" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="27" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -1716,7 +1736,615 @@
     <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
-  <dxfs count="39">
+  <dxfs count="99">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkUp">
+          <fgColor rgb="FF80CA3C"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkUp">
+          <fgColor rgb="FF80CA3C"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkUp">
+          <fgColor rgb="FF80CA3C"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkUp">
+          <fgColor rgb="FF80CA3C"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkUp">
+          <fgColor rgb="FF80CA3C"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkUp">
+          <fgColor rgb="FF80CA3C"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkUp">
+          <fgColor rgb="FF80CA3C"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkUp">
+          <fgColor rgb="FF80CA3C"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2117,15 +2745,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="38"/>
-      <tableStyleElement type="headerRow" dxfId="37"/>
-      <tableStyleElement type="totalRow" dxfId="36"/>
-      <tableStyleElement type="firstColumn" dxfId="35"/>
-      <tableStyleElement type="lastColumn" dxfId="34"/>
-      <tableStyleElement type="firstRowStripe" dxfId="33"/>
-      <tableStyleElement type="secondRowStripe" dxfId="32"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="31"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="30"/>
+      <tableStyleElement type="wholeTable" dxfId="98"/>
+      <tableStyleElement type="headerRow" dxfId="97"/>
+      <tableStyleElement type="totalRow" dxfId="96"/>
+      <tableStyleElement type="firstColumn" dxfId="95"/>
+      <tableStyleElement type="lastColumn" dxfId="94"/>
+      <tableStyleElement type="firstRowStripe" dxfId="93"/>
+      <tableStyleElement type="secondRowStripe" dxfId="92"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="91"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="90"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2541,23 +3169,23 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BQ24"/>
+  <dimension ref="A1:BQ25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="25" customWidth="1"/>
     <col min="2" max="2" width="34.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
     <col min="7" max="7" width="1.42578125" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" customWidth="1"/>
     <col min="9" max="64" width="2.5703125" customWidth="1"/>
     <col min="65" max="69" width="2.7109375" customWidth="1"/>
   </cols>
@@ -2592,1021 +3220,966 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:69" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+    <row r="3" spans="1:69" ht="3" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="26"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="14"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="10"/>
+      <c r="AL3" s="37"/>
+      <c r="AM3" s="32"/>
+      <c r="AW3" s="43"/>
+      <c r="AX3" s="43"/>
+    </row>
+    <row r="4" spans="1:69" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B4" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="28" t="s">
+      <c r="C4" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="107">
+        <f ca="1">D5-F4</f>
+        <v>-1.368896925858952E-2</v>
+      </c>
+      <c r="E4" s="105" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="106">
+        <f ca="1">(60-D6)/60</f>
+        <v>0.1</v>
+      </c>
+      <c r="I4" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="AL3" s="42"/>
-      <c r="AM3" s="42"/>
-      <c r="AN3" t="s">
+      <c r="AL4" s="42"/>
+      <c r="AM4" s="42"/>
+      <c r="AN4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:69" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4"/>
-      <c r="B4" s="25" t="s">
+    <row r="5" spans="1:69" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5"/>
+      <c r="B5" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C5" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="40">
-        <f ca="1">SUM(D9,D14)/2</f>
-        <v>5.5663527397260271E-2</v>
-      </c>
-      <c r="E4" s="93" t="s">
+      <c r="D5" s="40">
+        <f>SUM(D10,D15)/2</f>
+        <v>8.6311030741410485E-2</v>
+      </c>
+      <c r="E5" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="94">
+      <c r="F5" s="83">
         <f>DATE(2020, 6, 15)</f>
         <v>43997</v>
       </c>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
+      <c r="G5" s="111"/>
+      <c r="H5" s="111"/>
     </row>
-    <row r="5" spans="1:69" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5"/>
-      <c r="B5" s="26" t="s">
+    <row r="6" spans="1:69" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A6"/>
+      <c r="B6" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C6" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="41">
-        <f ca="1">DATEDIF(NOW(),BQ6,"D")</f>
-        <v>57</v>
-      </c>
-      <c r="E5" s="93" t="s">
+      <c r="D6" s="41">
+        <f ca="1">DATEDIF(NOW(),BQ7,"D")</f>
+        <v>54</v>
+      </c>
+      <c r="E6" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="95">
+      <c r="F6" s="84">
         <v>1</v>
       </c>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="119">
-        <f>I6</f>
+      <c r="G6" s="111"/>
+      <c r="H6" s="111"/>
+      <c r="I6" s="112">
+        <f>I7</f>
         <v>43997</v>
       </c>
-      <c r="J5" s="120"/>
-      <c r="K5" s="120"/>
-      <c r="L5" s="120"/>
-      <c r="M5" s="120"/>
-      <c r="N5" s="120"/>
-      <c r="O5" s="121"/>
-      <c r="P5" s="122">
-        <f>P6</f>
+      <c r="J6" s="109"/>
+      <c r="K6" s="109"/>
+      <c r="L6" s="109"/>
+      <c r="M6" s="109"/>
+      <c r="N6" s="109"/>
+      <c r="O6" s="113"/>
+      <c r="P6" s="108">
+        <f>P7</f>
         <v>44004</v>
       </c>
-      <c r="Q5" s="120"/>
-      <c r="R5" s="120"/>
-      <c r="S5" s="120"/>
-      <c r="T5" s="120"/>
-      <c r="U5" s="120"/>
-      <c r="V5" s="121"/>
-      <c r="W5" s="122">
-        <f>W6</f>
+      <c r="Q6" s="109"/>
+      <c r="R6" s="109"/>
+      <c r="S6" s="109"/>
+      <c r="T6" s="109"/>
+      <c r="U6" s="109"/>
+      <c r="V6" s="113"/>
+      <c r="W6" s="108">
+        <f>W7</f>
         <v>44011</v>
       </c>
-      <c r="X5" s="120"/>
-      <c r="Y5" s="120"/>
-      <c r="Z5" s="120"/>
-      <c r="AA5" s="120"/>
-      <c r="AB5" s="120"/>
-      <c r="AC5" s="121"/>
-      <c r="AD5" s="122">
-        <f>AD6</f>
+      <c r="X6" s="109"/>
+      <c r="Y6" s="109"/>
+      <c r="Z6" s="109"/>
+      <c r="AA6" s="109"/>
+      <c r="AB6" s="109"/>
+      <c r="AC6" s="113"/>
+      <c r="AD6" s="108">
+        <f>AD7</f>
         <v>44018</v>
       </c>
-      <c r="AE5" s="120"/>
-      <c r="AF5" s="120"/>
-      <c r="AG5" s="120"/>
-      <c r="AH5" s="120"/>
-      <c r="AI5" s="120"/>
-      <c r="AJ5" s="121"/>
-      <c r="AK5" s="122">
-        <f>AK6</f>
+      <c r="AE6" s="109"/>
+      <c r="AF6" s="109"/>
+      <c r="AG6" s="109"/>
+      <c r="AH6" s="109"/>
+      <c r="AI6" s="109"/>
+      <c r="AJ6" s="113"/>
+      <c r="AK6" s="108">
+        <f>AK7</f>
         <v>44025</v>
       </c>
-      <c r="AL5" s="120"/>
-      <c r="AM5" s="120"/>
-      <c r="AN5" s="120"/>
-      <c r="AO5" s="120"/>
-      <c r="AP5" s="120"/>
-      <c r="AQ5" s="121"/>
-      <c r="AR5" s="122">
-        <f>AR6</f>
+      <c r="AL6" s="109"/>
+      <c r="AM6" s="109"/>
+      <c r="AN6" s="109"/>
+      <c r="AO6" s="109"/>
+      <c r="AP6" s="109"/>
+      <c r="AQ6" s="113"/>
+      <c r="AR6" s="108">
+        <f>AR7</f>
         <v>44032</v>
       </c>
-      <c r="AS5" s="120"/>
-      <c r="AT5" s="120"/>
-      <c r="AU5" s="120"/>
-      <c r="AV5" s="120"/>
-      <c r="AW5" s="120"/>
-      <c r="AX5" s="121"/>
-      <c r="AY5" s="122">
-        <f>AY6</f>
+      <c r="AS6" s="109"/>
+      <c r="AT6" s="109"/>
+      <c r="AU6" s="109"/>
+      <c r="AV6" s="109"/>
+      <c r="AW6" s="109"/>
+      <c r="AX6" s="113"/>
+      <c r="AY6" s="108">
+        <f>AY7</f>
         <v>44039</v>
       </c>
-      <c r="AZ5" s="120"/>
-      <c r="BA5" s="120"/>
-      <c r="BB5" s="120"/>
-      <c r="BC5" s="120"/>
-      <c r="BD5" s="120"/>
-      <c r="BE5" s="121"/>
-      <c r="BF5" s="122">
-        <f>BF6</f>
+      <c r="AZ6" s="109"/>
+      <c r="BA6" s="109"/>
+      <c r="BB6" s="109"/>
+      <c r="BC6" s="109"/>
+      <c r="BD6" s="109"/>
+      <c r="BE6" s="113"/>
+      <c r="BF6" s="108">
+        <f>BF7</f>
         <v>44046</v>
       </c>
-      <c r="BG5" s="120"/>
-      <c r="BH5" s="120"/>
-      <c r="BI5" s="120"/>
-      <c r="BJ5" s="120"/>
-      <c r="BK5" s="120"/>
-      <c r="BL5" s="121"/>
-      <c r="BM5" s="122">
-        <f>BM6</f>
+      <c r="BG6" s="109"/>
+      <c r="BH6" s="109"/>
+      <c r="BI6" s="109"/>
+      <c r="BJ6" s="109"/>
+      <c r="BK6" s="109"/>
+      <c r="BL6" s="113"/>
+      <c r="BM6" s="108">
+        <f>BM7</f>
         <v>44053</v>
       </c>
-      <c r="BN5" s="120"/>
-      <c r="BO5" s="120"/>
-      <c r="BP5" s="120"/>
-      <c r="BQ5" s="123"/>
+      <c r="BN6" s="109"/>
+      <c r="BO6" s="109"/>
+      <c r="BP6" s="109"/>
+      <c r="BQ6" s="110"/>
     </row>
-    <row r="6" spans="1:69" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
+    <row r="7" spans="1:69" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="114"/>
-      <c r="C6" s="114"/>
-      <c r="D6" s="114"/>
-      <c r="E6" s="114"/>
-      <c r="F6" s="114"/>
-      <c r="G6" s="114"/>
-      <c r="I6" s="124">
+      <c r="B7" s="118"/>
+      <c r="C7" s="118"/>
+      <c r="D7" s="118"/>
+      <c r="E7" s="118"/>
+      <c r="F7" s="118"/>
+      <c r="G7" s="118"/>
+      <c r="I7" s="103">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>43997</v>
       </c>
-      <c r="J6" s="103">
-        <f>I6+1</f>
+      <c r="J7" s="90">
+        <f>I7+1</f>
         <v>43998</v>
       </c>
-      <c r="K6" s="103">
-        <f t="shared" ref="K6:AX6" si="0">J6+1</f>
+      <c r="K7" s="90">
+        <f t="shared" ref="K7:AX7" si="0">J7+1</f>
         <v>43999</v>
       </c>
-      <c r="L6" s="103">
+      <c r="L7" s="90">
         <f t="shared" si="0"/>
         <v>44000</v>
       </c>
-      <c r="M6" s="103">
+      <c r="M7" s="90">
         <f t="shared" si="0"/>
         <v>44001</v>
       </c>
-      <c r="N6" s="103">
+      <c r="N7" s="90">
         <f t="shared" si="0"/>
         <v>44002</v>
       </c>
-      <c r="O6" s="8">
+      <c r="O7" s="8">
         <f t="shared" si="0"/>
         <v>44003</v>
       </c>
-      <c r="P6" s="7">
-        <f>O6+1</f>
+      <c r="P7" s="7">
+        <f>O7+1</f>
         <v>44004</v>
       </c>
-      <c r="Q6" s="103">
-        <f>P6+1</f>
+      <c r="Q7" s="90">
+        <f>P7+1</f>
         <v>44005</v>
       </c>
-      <c r="R6" s="103">
+      <c r="R7" s="90">
         <f t="shared" si="0"/>
         <v>44006</v>
       </c>
-      <c r="S6" s="103">
+      <c r="S7" s="90">
         <f t="shared" si="0"/>
         <v>44007</v>
       </c>
-      <c r="T6" s="103">
+      <c r="T7" s="90">
         <f t="shared" si="0"/>
         <v>44008</v>
       </c>
-      <c r="U6" s="103">
+      <c r="U7" s="90">
         <f t="shared" si="0"/>
         <v>44009</v>
       </c>
-      <c r="V6" s="8">
+      <c r="V7" s="8">
         <f t="shared" si="0"/>
         <v>44010</v>
       </c>
-      <c r="W6" s="7">
-        <f>V6+1</f>
+      <c r="W7" s="7">
+        <f>V7+1</f>
         <v>44011</v>
       </c>
-      <c r="X6" s="103">
-        <f>W6+1</f>
+      <c r="X7" s="90">
+        <f>W7+1</f>
         <v>44012</v>
       </c>
-      <c r="Y6" s="125">
-        <f>X6+1</f>
+      <c r="Y7" s="104">
+        <f>X7+1</f>
         <v>44013</v>
       </c>
-      <c r="Z6" s="103">
+      <c r="Z7" s="90">
         <f t="shared" si="0"/>
         <v>44014</v>
       </c>
-      <c r="AA6" s="103">
+      <c r="AA7" s="90">
         <f t="shared" si="0"/>
         <v>44015</v>
       </c>
-      <c r="AB6" s="103">
+      <c r="AB7" s="90">
         <f t="shared" si="0"/>
         <v>44016</v>
       </c>
-      <c r="AC6" s="8">
+      <c r="AC7" s="8">
         <f t="shared" si="0"/>
         <v>44017</v>
       </c>
-      <c r="AD6" s="7">
-        <f>AC6+1</f>
+      <c r="AD7" s="7">
+        <f>AC7+1</f>
         <v>44018</v>
       </c>
-      <c r="AE6" s="103">
-        <f>AD6+1</f>
+      <c r="AE7" s="90">
+        <f>AD7+1</f>
         <v>44019</v>
       </c>
-      <c r="AF6" s="103">
+      <c r="AF7" s="90">
         <f t="shared" si="0"/>
         <v>44020</v>
       </c>
-      <c r="AG6" s="103">
+      <c r="AG7" s="90">
         <f t="shared" si="0"/>
         <v>44021</v>
       </c>
-      <c r="AH6" s="103">
+      <c r="AH7" s="90">
         <f t="shared" si="0"/>
         <v>44022</v>
       </c>
-      <c r="AI6" s="103">
+      <c r="AI7" s="90">
         <f t="shared" si="0"/>
         <v>44023</v>
       </c>
-      <c r="AJ6" s="8">
+      <c r="AJ7" s="8">
         <f t="shared" si="0"/>
         <v>44024</v>
       </c>
-      <c r="AK6" s="7">
-        <f>AJ6+1</f>
+      <c r="AK7" s="7">
+        <f>AJ7+1</f>
         <v>44025</v>
       </c>
-      <c r="AL6" s="103">
-        <f>AK6+1</f>
+      <c r="AL7" s="90">
+        <f>AK7+1</f>
         <v>44026</v>
       </c>
-      <c r="AM6" s="103">
+      <c r="AM7" s="90">
         <f t="shared" si="0"/>
         <v>44027</v>
       </c>
-      <c r="AN6" s="103">
+      <c r="AN7" s="90">
         <f t="shared" si="0"/>
         <v>44028</v>
       </c>
-      <c r="AO6" s="103">
+      <c r="AO7" s="90">
         <f t="shared" si="0"/>
         <v>44029</v>
       </c>
-      <c r="AP6" s="103">
+      <c r="AP7" s="90">
         <f t="shared" si="0"/>
         <v>44030</v>
       </c>
-      <c r="AQ6" s="8">
+      <c r="AQ7" s="8">
         <f t="shared" si="0"/>
         <v>44031</v>
       </c>
-      <c r="AR6" s="7">
-        <f>AQ6+1</f>
+      <c r="AR7" s="7">
+        <f>AQ7+1</f>
         <v>44032</v>
       </c>
-      <c r="AS6" s="103">
-        <f>AR6+1</f>
+      <c r="AS7" s="90">
+        <f>AR7+1</f>
         <v>44033</v>
       </c>
-      <c r="AT6" s="103">
+      <c r="AT7" s="90">
         <f t="shared" si="0"/>
         <v>44034</v>
       </c>
-      <c r="AU6" s="103">
+      <c r="AU7" s="90">
         <f t="shared" si="0"/>
         <v>44035</v>
       </c>
-      <c r="AV6" s="103">
+      <c r="AV7" s="90">
         <f t="shared" si="0"/>
         <v>44036</v>
       </c>
-      <c r="AW6" s="103">
+      <c r="AW7" s="90">
         <f t="shared" si="0"/>
         <v>44037</v>
       </c>
-      <c r="AX6" s="8">
+      <c r="AX7" s="8">
         <f t="shared" si="0"/>
         <v>44038</v>
       </c>
-      <c r="AY6" s="7">
-        <f>AX6+1</f>
+      <c r="AY7" s="7">
+        <f t="shared" ref="AY7:BQ7" si="1">AX7+1</f>
         <v>44039</v>
       </c>
-      <c r="AZ6" s="103">
-        <f>AY6+1</f>
+      <c r="AZ7" s="90">
+        <f t="shared" si="1"/>
         <v>44040</v>
       </c>
-      <c r="BA6" s="103">
-        <f t="shared" ref="BA6:BE6" si="1">AZ6+1</f>
+      <c r="BA7" s="90">
+        <f t="shared" si="1"/>
         <v>44041</v>
       </c>
-      <c r="BB6" s="103">
+      <c r="BB7" s="90">
         <f t="shared" si="1"/>
         <v>44042</v>
       </c>
-      <c r="BC6" s="103">
+      <c r="BC7" s="90">
         <f t="shared" si="1"/>
         <v>44043</v>
       </c>
-      <c r="BD6" s="103">
+      <c r="BD7" s="90">
         <f t="shared" si="1"/>
         <v>44044</v>
       </c>
-      <c r="BE6" s="8">
+      <c r="BE7" s="8">
         <f t="shared" si="1"/>
         <v>44045</v>
       </c>
-      <c r="BF6" s="7">
-        <f>BE6+1</f>
+      <c r="BF7" s="7">
+        <f t="shared" si="1"/>
         <v>44046</v>
       </c>
-      <c r="BG6" s="103">
-        <f>BF6+1</f>
+      <c r="BG7" s="90">
+        <f t="shared" si="1"/>
         <v>44047</v>
       </c>
-      <c r="BH6" s="103">
-        <f t="shared" ref="BH6:BL6" si="2">BG6+1</f>
+      <c r="BH7" s="90">
+        <f t="shared" si="1"/>
         <v>44048</v>
       </c>
-      <c r="BI6" s="103">
+      <c r="BI7" s="90">
+        <f t="shared" si="1"/>
+        <v>44049</v>
+      </c>
+      <c r="BJ7" s="90">
+        <f t="shared" si="1"/>
+        <v>44050</v>
+      </c>
+      <c r="BK7" s="90">
+        <f t="shared" si="1"/>
+        <v>44051</v>
+      </c>
+      <c r="BL7" s="8">
+        <f t="shared" si="1"/>
+        <v>44052</v>
+      </c>
+      <c r="BM7" s="7">
+        <f t="shared" si="1"/>
+        <v>44053</v>
+      </c>
+      <c r="BN7" s="90">
+        <f t="shared" si="1"/>
+        <v>44054</v>
+      </c>
+      <c r="BO7" s="90">
+        <f t="shared" si="1"/>
+        <v>44055</v>
+      </c>
+      <c r="BP7" s="90">
+        <f t="shared" si="1"/>
+        <v>44056</v>
+      </c>
+      <c r="BQ7" s="91">
+        <f t="shared" si="1"/>
+        <v>44057</v>
+      </c>
+    </row>
+    <row r="8" spans="1:69" ht="28.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="101" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="102"/>
+      <c r="D8" s="102" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="102" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="102" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="121" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="122"/>
+      <c r="I8" s="9" t="str">
+        <f>LEFT(TEXT(I7,"ddd"),1)</f>
+        <v>M</v>
+      </c>
+      <c r="J8" s="9" t="str">
+        <f t="shared" ref="J8:AR8" si="2">LEFT(TEXT(J7,"ddd"),1)</f>
+        <v>T</v>
+      </c>
+      <c r="K8" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>44049</v>
-      </c>
-      <c r="BJ6" s="103">
+        <v>W</v>
+      </c>
+      <c r="L8" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>44050</v>
-      </c>
-      <c r="BK6" s="103">
+        <v>T</v>
+      </c>
+      <c r="M8" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>44051</v>
-      </c>
-      <c r="BL6" s="8">
+        <v>F</v>
+      </c>
+      <c r="N8" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>44052</v>
-      </c>
-      <c r="BM6" s="7">
-        <f>BL6+1</f>
-        <v>44053</v>
-      </c>
-      <c r="BN6" s="103">
-        <f>BM6+1</f>
-        <v>44054</v>
-      </c>
-      <c r="BO6" s="103">
-        <f t="shared" ref="BO6" si="3">BN6+1</f>
-        <v>44055</v>
-      </c>
-      <c r="BP6" s="103">
-        <f t="shared" ref="BP6:BQ6" si="4">BO6+1</f>
-        <v>44056</v>
-      </c>
-      <c r="BQ6" s="104">
-        <f t="shared" si="4"/>
-        <v>44057</v>
+        <v>S</v>
+      </c>
+      <c r="O8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+      <c r="P8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>M</v>
+      </c>
+      <c r="Q8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>T</v>
+      </c>
+      <c r="R8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>W</v>
+      </c>
+      <c r="S8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>T</v>
+      </c>
+      <c r="T8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+      <c r="U8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+      <c r="V8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+      <c r="W8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>M</v>
+      </c>
+      <c r="X8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>T</v>
+      </c>
+      <c r="Y8" s="44" t="str">
+        <f>LEFT(TEXT(Y7,"ddd"),1)</f>
+        <v>W</v>
+      </c>
+      <c r="Z8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>T</v>
+      </c>
+      <c r="AA8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+      <c r="AB8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+      <c r="AC8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+      <c r="AD8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>M</v>
+      </c>
+      <c r="AE8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>T</v>
+      </c>
+      <c r="AF8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>W</v>
+      </c>
+      <c r="AG8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>T</v>
+      </c>
+      <c r="AH8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+      <c r="AI8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+      <c r="AJ8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+      <c r="AK8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>M</v>
+      </c>
+      <c r="AL8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>T</v>
+      </c>
+      <c r="AM8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>W</v>
+      </c>
+      <c r="AN8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>T</v>
+      </c>
+      <c r="AO8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+      <c r="AP8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+      <c r="AQ8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+      <c r="AR8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>M</v>
+      </c>
+      <c r="AS8" s="9" t="str">
+        <f t="shared" ref="AS8:BL8" si="3">LEFT(TEXT(AS7,"ddd"),1)</f>
+        <v>T</v>
+      </c>
+      <c r="AT8" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>W</v>
+      </c>
+      <c r="AU8" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>T</v>
+      </c>
+      <c r="AV8" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+      <c r="AW8" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>S</v>
+      </c>
+      <c r="AX8" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>S</v>
+      </c>
+      <c r="AY8" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>M</v>
+      </c>
+      <c r="AZ8" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>T</v>
+      </c>
+      <c r="BA8" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>W</v>
+      </c>
+      <c r="BB8" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>T</v>
+      </c>
+      <c r="BC8" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+      <c r="BD8" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>S</v>
+      </c>
+      <c r="BE8" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>S</v>
+      </c>
+      <c r="BF8" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>M</v>
+      </c>
+      <c r="BG8" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>T</v>
+      </c>
+      <c r="BH8" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>W</v>
+      </c>
+      <c r="BI8" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>T</v>
+      </c>
+      <c r="BJ8" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+      <c r="BK8" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>S</v>
+      </c>
+      <c r="BL8" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>S</v>
+      </c>
+      <c r="BM8" s="9" t="str">
+        <f>LEFT(TEXT(BM7,"ddd"),1)</f>
+        <v>M</v>
+      </c>
+      <c r="BN8" s="9" t="str">
+        <f>LEFT(TEXT(BN7,"ddd"),1)</f>
+        <v>T</v>
+      </c>
+      <c r="BO8" s="9" t="str">
+        <f>LEFT(TEXT(BO7,"ddd"),1)</f>
+        <v>W</v>
+      </c>
+      <c r="BP8" s="9" t="str">
+        <f>LEFT(TEXT(BP7,"ddd"),1)</f>
+        <v>T</v>
+      </c>
+      <c r="BQ8" s="92" t="str">
+        <f>LEFT(TEXT(BQ7,"ddd"),1)</f>
+        <v>F</v>
       </c>
     </row>
-    <row r="7" spans="1:69" ht="28.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="115" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="116"/>
-      <c r="D7" s="116" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="116" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="116" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" s="117" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" s="118"/>
-      <c r="I7" s="9" t="str">
-        <f t="shared" ref="I7" si="5">LEFT(TEXT(I6,"ddd"),1)</f>
-        <v>M</v>
-      </c>
-      <c r="J7" s="9" t="str">
-        <f t="shared" ref="J7:AR7" si="6">LEFT(TEXT(J6,"ddd"),1)</f>
-        <v>T</v>
-      </c>
-      <c r="K7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>W</v>
-      </c>
-      <c r="L7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>T</v>
-      </c>
-      <c r="M7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>F</v>
-      </c>
-      <c r="N7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>S</v>
-      </c>
-      <c r="O7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>S</v>
-      </c>
-      <c r="P7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>M</v>
-      </c>
-      <c r="Q7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>T</v>
-      </c>
-      <c r="R7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>W</v>
-      </c>
-      <c r="S7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>T</v>
-      </c>
-      <c r="T7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>F</v>
-      </c>
-      <c r="U7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>S</v>
-      </c>
-      <c r="V7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>S</v>
-      </c>
-      <c r="W7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>M</v>
-      </c>
-      <c r="X7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>T</v>
-      </c>
-      <c r="Y7" s="44" t="str">
-        <f t="shared" ref="Y7" si="7">LEFT(TEXT(Y6,"ddd"),1)</f>
-        <v>W</v>
-      </c>
-      <c r="Z7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>T</v>
-      </c>
-      <c r="AA7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>F</v>
-      </c>
-      <c r="AB7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>S</v>
-      </c>
-      <c r="AC7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>S</v>
-      </c>
-      <c r="AD7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>M</v>
-      </c>
-      <c r="AE7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>T</v>
-      </c>
-      <c r="AF7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>W</v>
-      </c>
-      <c r="AG7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>T</v>
-      </c>
-      <c r="AH7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>F</v>
-      </c>
-      <c r="AI7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>S</v>
-      </c>
-      <c r="AJ7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>S</v>
-      </c>
-      <c r="AK7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>M</v>
-      </c>
-      <c r="AL7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>T</v>
-      </c>
-      <c r="AM7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>W</v>
-      </c>
-      <c r="AN7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>T</v>
-      </c>
-      <c r="AO7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>F</v>
-      </c>
-      <c r="AP7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>S</v>
-      </c>
-      <c r="AQ7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>S</v>
-      </c>
-      <c r="AR7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>M</v>
-      </c>
-      <c r="AS7" s="9" t="str">
-        <f t="shared" ref="AS7:BL7" si="8">LEFT(TEXT(AS6,"ddd"),1)</f>
-        <v>T</v>
-      </c>
-      <c r="AT7" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>W</v>
-      </c>
-      <c r="AU7" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>T</v>
-      </c>
-      <c r="AV7" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>F</v>
-      </c>
-      <c r="AW7" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>S</v>
-      </c>
-      <c r="AX7" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>S</v>
-      </c>
-      <c r="AY7" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>M</v>
-      </c>
-      <c r="AZ7" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>T</v>
-      </c>
-      <c r="BA7" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>W</v>
-      </c>
-      <c r="BB7" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>T</v>
-      </c>
-      <c r="BC7" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>F</v>
-      </c>
-      <c r="BD7" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>S</v>
-      </c>
-      <c r="BE7" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>S</v>
-      </c>
-      <c r="BF7" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>M</v>
-      </c>
-      <c r="BG7" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>T</v>
-      </c>
-      <c r="BH7" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>W</v>
-      </c>
-      <c r="BI7" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>T</v>
-      </c>
-      <c r="BJ7" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>F</v>
-      </c>
-      <c r="BK7" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>S</v>
-      </c>
-      <c r="BL7" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>S</v>
-      </c>
-      <c r="BM7" s="9" t="str">
-        <f t="shared" ref="BM7:BP7" si="9">LEFT(TEXT(BM6,"ddd"),1)</f>
-        <v>M</v>
-      </c>
-      <c r="BN7" s="9" t="str">
-        <f t="shared" si="9"/>
-        <v>T</v>
-      </c>
-      <c r="BO7" s="9" t="str">
-        <f t="shared" si="9"/>
-        <v>W</v>
-      </c>
-      <c r="BP7" s="9" t="str">
-        <f t="shared" si="9"/>
-        <v>T</v>
-      </c>
-      <c r="BQ7" s="105" t="str">
-        <f t="shared" ref="BQ7" si="10">LEFT(TEXT(BQ6,"ddd"),1)</f>
-        <v>F</v>
-      </c>
-    </row>
-    <row r="8" spans="1:69" ht="7.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="25" t="s">
+    <row r="9" spans="1:69" ht="7.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="111"/>
-      <c r="C8" s="29"/>
-      <c r="E8"/>
-      <c r="H8" t="str">
+      <c r="B9" s="98"/>
+      <c r="C9" s="29"/>
+      <c r="E9"/>
+      <c r="H9" t="str">
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
-      <c r="I8" s="72"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="72"/>
-      <c r="L8" s="72"/>
-      <c r="M8" s="72"/>
-      <c r="N8" s="72"/>
-      <c r="O8" s="72"/>
-      <c r="P8" s="72"/>
-      <c r="Q8" s="72"/>
-      <c r="R8" s="72"/>
-      <c r="S8" s="72"/>
-      <c r="T8" s="72"/>
-      <c r="U8" s="72"/>
-      <c r="V8" s="72"/>
-      <c r="W8" s="72"/>
-      <c r="X8" s="72"/>
-      <c r="Y8" s="72"/>
-      <c r="Z8" s="72"/>
-      <c r="AA8" s="72"/>
-      <c r="AB8" s="72"/>
-      <c r="AC8" s="72"/>
-      <c r="AD8" s="72"/>
-      <c r="AE8" s="72"/>
-      <c r="AF8" s="72"/>
-      <c r="AG8" s="72"/>
-      <c r="AH8" s="72"/>
-      <c r="AI8" s="72"/>
-      <c r="AJ8" s="72"/>
-      <c r="AK8" s="72"/>
-      <c r="AL8" s="72"/>
-      <c r="AM8" s="72"/>
-      <c r="AN8" s="72"/>
-      <c r="AO8" s="72"/>
-      <c r="AP8" s="72"/>
-      <c r="AQ8" s="72"/>
-      <c r="AR8" s="72"/>
-      <c r="AS8" s="72"/>
-      <c r="AT8" s="72"/>
-      <c r="AU8" s="72"/>
-      <c r="AV8" s="72"/>
-      <c r="AW8" s="72"/>
-      <c r="AX8" s="72"/>
-      <c r="AY8" s="72"/>
-      <c r="AZ8" s="72"/>
-      <c r="BA8" s="72"/>
-      <c r="BB8" s="72"/>
-      <c r="BC8" s="72"/>
-      <c r="BD8" s="72"/>
-      <c r="BE8" s="72"/>
-      <c r="BF8" s="72"/>
-      <c r="BG8" s="72"/>
-      <c r="BH8" s="72"/>
-      <c r="BI8" s="72"/>
-      <c r="BJ8" s="72"/>
-      <c r="BK8" s="72"/>
-      <c r="BL8" s="72"/>
-      <c r="BM8" s="72"/>
-      <c r="BN8" s="72"/>
-      <c r="BO8" s="72"/>
-      <c r="BP8" s="72"/>
-      <c r="BQ8" s="45"/>
-    </row>
-    <row r="9" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="112" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="78"/>
-      <c r="D9" s="91">
-        <f ca="1">(D10*DATEDIF(E10,F10,"D")+D11*DATEDIF(E11,F11,"D")+D12*DATEDIF(E12,F12,"D")+D13*DATEDIF(E13,F13,"D"))/(DATEDIF(E10,F10,"D")+DATEDIF(E11,F11,"D")+DATEDIF(E12,F12,"D")+DATEDIF(E13,F13,"D"))</f>
-        <v>7.9452054794520541E-2</v>
-      </c>
-      <c r="E9" s="79"/>
-      <c r="F9" s="80"/>
-      <c r="G9" s="80"/>
-      <c r="H9" s="80"/>
-      <c r="I9" s="80"/>
-      <c r="J9" s="80"/>
-      <c r="K9" s="80"/>
-      <c r="L9" s="80"/>
-      <c r="M9" s="80"/>
-      <c r="N9" s="80"/>
-      <c r="O9" s="80"/>
-      <c r="P9" s="80"/>
-      <c r="Q9" s="80"/>
-      <c r="R9" s="80"/>
-      <c r="S9" s="80"/>
-      <c r="T9" s="80"/>
-      <c r="U9" s="80"/>
-      <c r="V9" s="80"/>
-      <c r="W9" s="80"/>
-      <c r="X9" s="80"/>
-      <c r="Y9" s="80"/>
-      <c r="Z9" s="80"/>
-      <c r="AA9" s="80"/>
-      <c r="AB9" s="80"/>
-      <c r="AC9" s="80"/>
-      <c r="AD9" s="80"/>
-      <c r="AE9" s="78"/>
-      <c r="AF9" s="81"/>
-      <c r="AG9" s="79"/>
-      <c r="AH9" s="80"/>
-      <c r="AI9" s="80"/>
-      <c r="AJ9" s="80"/>
-      <c r="AK9" s="80"/>
-      <c r="AL9" s="80"/>
-      <c r="AM9" s="80"/>
-      <c r="AN9" s="80"/>
-      <c r="AO9" s="80"/>
-      <c r="AP9" s="80"/>
-      <c r="AQ9" s="80"/>
-      <c r="AR9" s="80"/>
-      <c r="AS9" s="80"/>
-      <c r="AT9" s="80"/>
-      <c r="AU9" s="80"/>
-      <c r="AV9" s="80"/>
-      <c r="AW9" s="80"/>
-      <c r="AX9" s="80"/>
-      <c r="AY9" s="80"/>
-      <c r="AZ9" s="80"/>
-      <c r="BA9" s="80"/>
-      <c r="BB9" s="80"/>
-      <c r="BC9" s="80"/>
-      <c r="BD9" s="80"/>
-      <c r="BE9" s="80"/>
-      <c r="BF9" s="80"/>
-      <c r="BG9" s="78"/>
-      <c r="BH9" s="81"/>
-      <c r="BI9" s="79"/>
-      <c r="BJ9" s="80"/>
-      <c r="BK9" s="80"/>
-      <c r="BL9" s="80"/>
-      <c r="BM9" s="80"/>
-      <c r="BN9" s="80"/>
-      <c r="BO9" s="80"/>
-      <c r="BP9" s="80"/>
-      <c r="BQ9" s="106"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="63"/>
+      <c r="N9" s="63"/>
+      <c r="O9" s="63"/>
+      <c r="P9" s="63"/>
+      <c r="Q9" s="63"/>
+      <c r="R9" s="63"/>
+      <c r="S9" s="63"/>
+      <c r="T9" s="63"/>
+      <c r="U9" s="63"/>
+      <c r="V9" s="63"/>
+      <c r="W9" s="63"/>
+      <c r="X9" s="63"/>
+      <c r="Y9" s="63"/>
+      <c r="Z9" s="63"/>
+      <c r="AA9" s="63"/>
+      <c r="AB9" s="63"/>
+      <c r="AC9" s="63"/>
+      <c r="AD9" s="63"/>
+      <c r="AE9" s="63"/>
+      <c r="AF9" s="63"/>
+      <c r="AG9" s="63"/>
+      <c r="AH9" s="63"/>
+      <c r="AI9" s="63"/>
+      <c r="AJ9" s="63"/>
+      <c r="AK9" s="63"/>
+      <c r="AL9" s="63"/>
+      <c r="AM9" s="63"/>
+      <c r="AN9" s="63"/>
+      <c r="AO9" s="63"/>
+      <c r="AP9" s="63"/>
+      <c r="AQ9" s="63"/>
+      <c r="AR9" s="63"/>
+      <c r="AS9" s="63"/>
+      <c r="AT9" s="63"/>
+      <c r="AU9" s="63"/>
+      <c r="AV9" s="63"/>
+      <c r="AW9" s="63"/>
+      <c r="AX9" s="63"/>
+      <c r="AY9" s="63"/>
+      <c r="AZ9" s="63"/>
+      <c r="BA9" s="63"/>
+      <c r="BB9" s="63"/>
+      <c r="BC9" s="63"/>
+      <c r="BD9" s="63"/>
+      <c r="BE9" s="63"/>
+      <c r="BF9" s="63"/>
+      <c r="BG9" s="63"/>
+      <c r="BH9" s="63"/>
+      <c r="BI9" s="63"/>
+      <c r="BJ9" s="63"/>
+      <c r="BK9" s="63"/>
+      <c r="BL9" s="63"/>
+      <c r="BM9" s="63"/>
+      <c r="BN9" s="63"/>
+      <c r="BO9" s="63"/>
+      <c r="BP9" s="63"/>
+      <c r="BQ9" s="45"/>
     </row>
     <row r="10" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="25"/>
-      <c r="B10" s="136" t="s">
+      <c r="A10" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="99" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="68"/>
+      <c r="D10" s="80">
+        <f>(D12*DATEDIF(E12,F12,"D")+D13*DATEDIF(E13,F13,"D")+D14*DATEDIF(E14,F14,"D"))/(DATEDIF(E12,F12,"D")+DATEDIF(E13,F13,"D")+DATEDIF(E14,F14,"D"))</f>
+        <v>0.12857142857142856</v>
+      </c>
+      <c r="E10" s="69"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="141">
+        <f ca="1">DATEDIF(E11,NOW(), "D")/DATEDIF(E11,F14,"d")</f>
+        <v>0.4</v>
+      </c>
+      <c r="H10" s="141"/>
+      <c r="I10" s="70"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="70"/>
+      <c r="L10" s="70"/>
+      <c r="M10" s="70"/>
+      <c r="N10" s="70"/>
+      <c r="O10" s="70"/>
+      <c r="P10" s="70"/>
+      <c r="Q10" s="70"/>
+      <c r="R10" s="70"/>
+      <c r="S10" s="70"/>
+      <c r="T10" s="70"/>
+      <c r="U10" s="70"/>
+      <c r="V10" s="70"/>
+      <c r="W10" s="70"/>
+      <c r="X10" s="70"/>
+      <c r="Y10" s="70"/>
+      <c r="Z10" s="70"/>
+      <c r="AA10" s="70"/>
+      <c r="AB10" s="70"/>
+      <c r="AC10" s="70"/>
+      <c r="AD10" s="70"/>
+      <c r="AE10" s="68"/>
+      <c r="AF10" s="71"/>
+      <c r="AG10" s="69"/>
+      <c r="AH10" s="70"/>
+      <c r="AI10" s="70"/>
+      <c r="AJ10" s="70"/>
+      <c r="AK10" s="70"/>
+      <c r="AL10" s="70"/>
+      <c r="AM10" s="70"/>
+      <c r="AN10" s="70"/>
+      <c r="AO10" s="70"/>
+      <c r="AP10" s="70"/>
+      <c r="AQ10" s="70"/>
+      <c r="AR10" s="70"/>
+      <c r="AS10" s="70"/>
+      <c r="AT10" s="70"/>
+      <c r="AU10" s="70"/>
+      <c r="AV10" s="70"/>
+      <c r="AW10" s="70"/>
+      <c r="AX10" s="70"/>
+      <c r="AY10" s="70"/>
+      <c r="AZ10" s="70"/>
+      <c r="BA10" s="70"/>
+      <c r="BB10" s="70"/>
+      <c r="BC10" s="70"/>
+      <c r="BD10" s="70"/>
+      <c r="BE10" s="70"/>
+      <c r="BF10" s="70"/>
+      <c r="BG10" s="68"/>
+      <c r="BH10" s="71"/>
+      <c r="BI10" s="69"/>
+      <c r="BJ10" s="70"/>
+      <c r="BK10" s="70"/>
+      <c r="BL10" s="70"/>
+      <c r="BM10" s="70"/>
+      <c r="BN10" s="70"/>
+      <c r="BO10" s="70"/>
+      <c r="BP10" s="70"/>
+      <c r="BQ10" s="93"/>
+    </row>
+    <row r="11" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="25"/>
+      <c r="B11" s="135" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="137"/>
-      <c r="D10" s="73">
-        <f ca="1">(60-DATEDIF(NOW(),F10,"D"))/59</f>
-        <v>6.7796610169491525E-2</v>
-      </c>
-      <c r="E10" s="82">
+      <c r="C11" s="136"/>
+      <c r="D11" s="64">
+        <f ca="1">(60-DATEDIF(NOW(),F11,"D"))/59</f>
+        <v>0.11864406779661017</v>
+      </c>
+      <c r="E11" s="72">
         <f>Project_Start</f>
         <v>43997</v>
       </c>
-      <c r="F10" s="86">
-        <f>E10+59</f>
+      <c r="F11" s="75">
+        <f>E11+59</f>
         <v>44056</v>
       </c>
-      <c r="G10" s="52">
-        <f t="shared" ref="G10:H21" si="11">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+      <c r="G11" s="137">
+        <f t="shared" ref="G11:G22" si="4">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v>60</v>
       </c>
-      <c r="H10" s="74"/>
-      <c r="I10" s="75"/>
-      <c r="J10" s="76"/>
-      <c r="K10" s="76"/>
-      <c r="L10" s="76"/>
-      <c r="M10" s="76"/>
-      <c r="N10" s="76"/>
-      <c r="O10" s="76"/>
-      <c r="P10" s="76"/>
-      <c r="Q10" s="76"/>
-      <c r="R10" s="76"/>
-      <c r="S10" s="76"/>
-      <c r="T10" s="76"/>
-      <c r="U10" s="76"/>
-      <c r="V10" s="76"/>
-      <c r="W10" s="76"/>
-      <c r="X10" s="76"/>
-      <c r="Y10" s="46"/>
-      <c r="Z10" s="76"/>
-      <c r="AA10" s="76"/>
-      <c r="AB10" s="76"/>
-      <c r="AC10" s="76"/>
-      <c r="AD10" s="76"/>
-      <c r="AE10" s="76"/>
-      <c r="AF10" s="76"/>
-      <c r="AG10" s="76"/>
-      <c r="AH10" s="76"/>
-      <c r="AI10" s="76"/>
-      <c r="AJ10" s="76"/>
-      <c r="AK10" s="76"/>
-      <c r="AL10" s="76"/>
-      <c r="AM10" s="76"/>
-      <c r="AN10" s="76"/>
-      <c r="AO10" s="76"/>
-      <c r="AP10" s="76"/>
-      <c r="AQ10" s="76"/>
-      <c r="AR10" s="76"/>
-      <c r="AS10" s="76"/>
-      <c r="AT10" s="76"/>
-      <c r="AU10" s="76"/>
-      <c r="AV10" s="76"/>
-      <c r="AW10" s="76"/>
-      <c r="AX10" s="76"/>
-      <c r="AY10" s="76"/>
-      <c r="AZ10" s="76"/>
-      <c r="BA10" s="76"/>
-      <c r="BB10" s="76"/>
-      <c r="BC10" s="76"/>
-      <c r="BD10" s="76"/>
-      <c r="BE10" s="76"/>
-      <c r="BF10" s="76"/>
-      <c r="BG10" s="76"/>
-      <c r="BH10" s="76"/>
-      <c r="BI10" s="76"/>
-      <c r="BJ10" s="76"/>
-      <c r="BK10" s="76"/>
-      <c r="BL10" s="76"/>
-      <c r="BM10" s="76"/>
-      <c r="BN10" s="76"/>
-      <c r="BO10" s="76"/>
-      <c r="BP10" s="77"/>
-      <c r="BQ10" s="107"/>
-    </row>
-    <row r="11" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="134" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="135"/>
-      <c r="D11" s="12">
-        <v>0.3</v>
-      </c>
-      <c r="E11" s="83">
-        <f>Project_Start</f>
-        <v>43997</v>
-      </c>
-      <c r="F11" s="87">
-        <f>E11+6</f>
-        <v>44003</v>
-      </c>
-      <c r="G11" s="85">
-        <f t="shared" si="11"/>
-        <v>7</v>
-      </c>
-      <c r="H11" s="50"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="33"/>
-      <c r="O11" s="33"/>
-      <c r="P11" s="33"/>
-      <c r="Q11" s="33"/>
-      <c r="R11" s="33"/>
-      <c r="S11" s="33"/>
-      <c r="T11" s="33"/>
-      <c r="U11" s="33"/>
-      <c r="V11" s="33"/>
-      <c r="W11" s="33"/>
-      <c r="X11" s="33"/>
-      <c r="Y11" s="45"/>
-      <c r="Z11" s="33"/>
-      <c r="AA11" s="33"/>
-      <c r="AB11" s="33"/>
-      <c r="AC11" s="33"/>
-      <c r="AD11" s="33"/>
-      <c r="AE11" s="33"/>
-      <c r="AF11" s="33"/>
-      <c r="AG11" s="33"/>
-      <c r="AH11" s="33"/>
-      <c r="AI11" s="33"/>
-      <c r="AJ11" s="33"/>
-      <c r="AK11" s="33"/>
-      <c r="AL11" s="33"/>
-      <c r="AM11" s="33"/>
-      <c r="AN11" s="33"/>
-      <c r="AO11" s="33"/>
-      <c r="AP11" s="33"/>
-      <c r="AQ11" s="33"/>
-      <c r="AR11" s="33"/>
-      <c r="AS11" s="33"/>
-      <c r="AT11" s="33"/>
-      <c r="AU11" s="33"/>
-      <c r="AV11" s="33"/>
-      <c r="AW11" s="33"/>
-      <c r="AX11" s="33"/>
-      <c r="AY11" s="33"/>
-      <c r="AZ11" s="33"/>
-      <c r="BA11" s="33"/>
-      <c r="BB11" s="33"/>
-      <c r="BC11" s="33"/>
-      <c r="BD11" s="33"/>
-      <c r="BE11" s="33"/>
-      <c r="BF11" s="33"/>
-      <c r="BG11" s="33"/>
-      <c r="BH11" s="33"/>
-      <c r="BI11" s="33"/>
-      <c r="BJ11" s="33"/>
-      <c r="BK11" s="33"/>
-      <c r="BL11" s="33"/>
-      <c r="BM11" s="33"/>
-      <c r="BN11" s="33"/>
-      <c r="BO11" s="33"/>
-      <c r="BP11" s="33"/>
-      <c r="BQ11" s="108"/>
+      <c r="H11" s="138"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="66"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="66"/>
+      <c r="M11" s="66"/>
+      <c r="N11" s="66"/>
+      <c r="O11" s="66"/>
+      <c r="P11" s="66"/>
+      <c r="Q11" s="66"/>
+      <c r="R11" s="66"/>
+      <c r="S11" s="66"/>
+      <c r="T11" s="66"/>
+      <c r="U11" s="66"/>
+      <c r="V11" s="66"/>
+      <c r="W11" s="66"/>
+      <c r="X11" s="66"/>
+      <c r="Y11" s="46"/>
+      <c r="Z11" s="66"/>
+      <c r="AA11" s="66"/>
+      <c r="AB11" s="66"/>
+      <c r="AC11" s="66"/>
+      <c r="AD11" s="66"/>
+      <c r="AE11" s="66"/>
+      <c r="AF11" s="66"/>
+      <c r="AG11" s="66"/>
+      <c r="AH11" s="66"/>
+      <c r="AI11" s="66"/>
+      <c r="AJ11" s="66"/>
+      <c r="AK11" s="66"/>
+      <c r="AL11" s="66"/>
+      <c r="AM11" s="66"/>
+      <c r="AN11" s="66"/>
+      <c r="AO11" s="66"/>
+      <c r="AP11" s="66"/>
+      <c r="AQ11" s="66"/>
+      <c r="AR11" s="66"/>
+      <c r="AS11" s="66"/>
+      <c r="AT11" s="66"/>
+      <c r="AU11" s="66"/>
+      <c r="AV11" s="66"/>
+      <c r="AW11" s="66"/>
+      <c r="AX11" s="66"/>
+      <c r="AY11" s="66"/>
+      <c r="AZ11" s="66"/>
+      <c r="BA11" s="66"/>
+      <c r="BB11" s="66"/>
+      <c r="BC11" s="66"/>
+      <c r="BD11" s="66"/>
+      <c r="BE11" s="66"/>
+      <c r="BF11" s="66"/>
+      <c r="BG11" s="66"/>
+      <c r="BH11" s="66"/>
+      <c r="BI11" s="66"/>
+      <c r="BJ11" s="66"/>
+      <c r="BK11" s="66"/>
+      <c r="BL11" s="66"/>
+      <c r="BM11" s="66"/>
+      <c r="BN11" s="66"/>
+      <c r="BO11" s="66"/>
+      <c r="BP11" s="67"/>
+      <c r="BQ11" s="94"/>
     </row>
     <row r="12" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="134" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="135"/>
+        <v>30</v>
+      </c>
+      <c r="B12" s="131" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="132"/>
       <c r="D12" s="12">
-        <v>0</v>
-      </c>
-      <c r="E12" s="83">
-        <f>F11+1</f>
-        <v>44004</v>
-      </c>
-      <c r="F12" s="87">
-        <f>E12+1</f>
-        <v>44005</v>
-      </c>
-      <c r="G12" s="85">
-        <f t="shared" si="11"/>
-        <v>2</v>
-      </c>
-      <c r="H12" s="50"/>
-      <c r="I12" s="47"/>
+        <v>0.3</v>
+      </c>
+      <c r="E12" s="73">
+        <f>Project_Start</f>
+        <v>43997</v>
+      </c>
+      <c r="F12" s="76">
+        <f>E12+6</f>
+        <v>44003</v>
+      </c>
+      <c r="G12" s="139">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="H12" s="140"/>
+      <c r="I12" s="48"/>
       <c r="J12" s="33"/>
       <c r="K12" s="33"/>
       <c r="L12" s="33"/>
@@ -3618,8 +4191,8 @@
       <c r="R12" s="33"/>
       <c r="S12" s="33"/>
       <c r="T12" s="33"/>
-      <c r="U12" s="34"/>
-      <c r="V12" s="34"/>
+      <c r="U12" s="33"/>
+      <c r="V12" s="33"/>
       <c r="W12" s="33"/>
       <c r="X12" s="33"/>
       <c r="Y12" s="45"/>
@@ -3666,359 +4239,364 @@
       <c r="BN12" s="33"/>
       <c r="BO12" s="33"/>
       <c r="BP12" s="33"/>
-      <c r="BQ12" s="108"/>
+      <c r="BQ12" s="95"/>
     </row>
     <row r="13" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="25"/>
-      <c r="B13" s="132" t="s">
+      <c r="A13" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="131" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="132"/>
+      <c r="D13" s="12">
+        <v>0</v>
+      </c>
+      <c r="E13" s="73">
+        <f>F12+1</f>
+        <v>44004</v>
+      </c>
+      <c r="F13" s="76">
+        <f>E13+1</f>
+        <v>44005</v>
+      </c>
+      <c r="G13" s="139">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="H13" s="140"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="33"/>
+      <c r="O13" s="33"/>
+      <c r="P13" s="33"/>
+      <c r="Q13" s="33"/>
+      <c r="R13" s="33"/>
+      <c r="S13" s="33"/>
+      <c r="T13" s="33"/>
+      <c r="U13" s="34"/>
+      <c r="V13" s="34"/>
+      <c r="W13" s="33"/>
+      <c r="X13" s="33"/>
+      <c r="Y13" s="45"/>
+      <c r="Z13" s="33"/>
+      <c r="AA13" s="33"/>
+      <c r="AB13" s="33"/>
+      <c r="AC13" s="33"/>
+      <c r="AD13" s="33"/>
+      <c r="AE13" s="33"/>
+      <c r="AF13" s="33"/>
+      <c r="AG13" s="33"/>
+      <c r="AH13" s="33"/>
+      <c r="AI13" s="33"/>
+      <c r="AJ13" s="33"/>
+      <c r="AK13" s="33"/>
+      <c r="AL13" s="33"/>
+      <c r="AM13" s="33"/>
+      <c r="AN13" s="33"/>
+      <c r="AO13" s="33"/>
+      <c r="AP13" s="33"/>
+      <c r="AQ13" s="33"/>
+      <c r="AR13" s="33"/>
+      <c r="AS13" s="33"/>
+      <c r="AT13" s="33"/>
+      <c r="AU13" s="33"/>
+      <c r="AV13" s="33"/>
+      <c r="AW13" s="33"/>
+      <c r="AX13" s="33"/>
+      <c r="AY13" s="33"/>
+      <c r="AZ13" s="33"/>
+      <c r="BA13" s="33"/>
+      <c r="BB13" s="33"/>
+      <c r="BC13" s="33"/>
+      <c r="BD13" s="33"/>
+      <c r="BE13" s="33"/>
+      <c r="BF13" s="33"/>
+      <c r="BG13" s="33"/>
+      <c r="BH13" s="33"/>
+      <c r="BI13" s="33"/>
+      <c r="BJ13" s="33"/>
+      <c r="BK13" s="33"/>
+      <c r="BL13" s="33"/>
+      <c r="BM13" s="33"/>
+      <c r="BN13" s="33"/>
+      <c r="BO13" s="33"/>
+      <c r="BP13" s="33"/>
+      <c r="BQ13" s="95"/>
+    </row>
+    <row r="14" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="25"/>
+      <c r="B14" s="129" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="133"/>
-      <c r="D13" s="56">
+      <c r="C14" s="130"/>
+      <c r="D14" s="50">
         <v>0</v>
       </c>
-      <c r="E13" s="84">
-        <f>E12+1</f>
+      <c r="E14" s="74">
+        <f>E13+1</f>
         <v>44005</v>
       </c>
-      <c r="F13" s="88">
-        <f>E13+7</f>
+      <c r="F14" s="77">
+        <f>E14+7</f>
         <v>44012</v>
       </c>
-      <c r="G13" s="51">
-        <f t="shared" si="11"/>
+      <c r="G14" s="133">
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="H13" s="57"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59"/>
-      <c r="N13" s="59"/>
-      <c r="O13" s="59"/>
-      <c r="P13" s="59"/>
-      <c r="Q13" s="60"/>
-      <c r="R13" s="59"/>
-      <c r="S13" s="59"/>
-      <c r="T13" s="59"/>
-      <c r="U13" s="59"/>
-      <c r="V13" s="59"/>
-      <c r="W13" s="59"/>
-      <c r="X13" s="59"/>
-      <c r="Y13" s="45"/>
-      <c r="Z13" s="59"/>
-      <c r="AA13" s="59"/>
-      <c r="AB13" s="59"/>
-      <c r="AC13" s="59"/>
-      <c r="AD13" s="59"/>
-      <c r="AE13" s="59"/>
-      <c r="AF13" s="59"/>
-      <c r="AG13" s="59"/>
-      <c r="AH13" s="59"/>
-      <c r="AI13" s="59"/>
-      <c r="AJ13" s="59"/>
-      <c r="AK13" s="59"/>
-      <c r="AL13" s="59"/>
-      <c r="AM13" s="59"/>
-      <c r="AN13" s="59"/>
-      <c r="AO13" s="59"/>
-      <c r="AP13" s="59"/>
-      <c r="AQ13" s="59"/>
-      <c r="AR13" s="59"/>
-      <c r="AS13" s="59"/>
-      <c r="AT13" s="59"/>
-      <c r="AU13" s="59"/>
-      <c r="AV13" s="59"/>
-      <c r="AW13" s="59"/>
-      <c r="AX13" s="59"/>
-      <c r="AY13" s="59"/>
-      <c r="AZ13" s="59"/>
-      <c r="BA13" s="59"/>
-      <c r="BB13" s="59"/>
-      <c r="BC13" s="59"/>
-      <c r="BD13" s="59"/>
-      <c r="BE13" s="59"/>
-      <c r="BF13" s="59"/>
-      <c r="BG13" s="59"/>
-      <c r="BH13" s="59"/>
-      <c r="BI13" s="59"/>
-      <c r="BJ13" s="59"/>
-      <c r="BK13" s="59"/>
-      <c r="BL13" s="59"/>
-      <c r="BM13" s="59"/>
-      <c r="BN13" s="59"/>
-      <c r="BO13" s="59"/>
-      <c r="BP13" s="59"/>
-      <c r="BQ13" s="108"/>
-    </row>
-    <row r="14" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="113" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="66"/>
-      <c r="D14" s="67">
-        <f>(D15*DATEDIF(E15,F15,"D")+D16*DATEDIF(E16,F16,"D")+D17*DATEDIF(E17,F17,"D")+D18*DATEDIF(E18,F18,"D")+D19*DATEDIF(E19,F19,"D")+D20*DATEDIF(E20,F20,"D")+D21*DATEDIF(E21,F21,"D"))/(DATEDIF(E15,F15,"D")+DATEDIF(E16,F16,"D")+DATEDIF(E17,F17,"D")+DATEDIF(E18,F18,"D")+DATEDIF(E19,F19,"D")+DATEDIF(E20,F20,"D")+DATEDIF(E21,F21,"D"))</f>
-        <v>3.1875000000000001E-2</v>
-      </c>
-      <c r="E14" s="68"/>
-      <c r="F14" s="69"/>
-      <c r="G14" s="70"/>
-      <c r="H14" s="70"/>
-      <c r="I14" s="70"/>
-      <c r="J14" s="70"/>
-      <c r="K14" s="70"/>
-      <c r="L14" s="70"/>
-      <c r="M14" s="70"/>
-      <c r="N14" s="70"/>
-      <c r="O14" s="70"/>
-      <c r="P14" s="70"/>
-      <c r="Q14" s="70"/>
-      <c r="R14" s="70"/>
-      <c r="S14" s="70"/>
-      <c r="T14" s="70"/>
-      <c r="U14" s="70"/>
-      <c r="V14" s="70"/>
-      <c r="W14" s="70"/>
-      <c r="X14" s="70"/>
-      <c r="Y14" s="92"/>
-      <c r="Z14" s="70"/>
-      <c r="AA14" s="70"/>
-      <c r="AB14" s="70"/>
-      <c r="AC14" s="70"/>
-      <c r="AD14" s="70"/>
-      <c r="AE14" s="70"/>
-      <c r="AF14" s="70"/>
-      <c r="AG14" s="70"/>
-      <c r="AH14" s="70"/>
-      <c r="AI14" s="70"/>
-      <c r="AJ14" s="70"/>
-      <c r="AK14" s="70"/>
-      <c r="AL14" s="70"/>
-      <c r="AM14" s="70"/>
-      <c r="AN14" s="70"/>
-      <c r="AO14" s="70"/>
-      <c r="AP14" s="70"/>
-      <c r="AQ14" s="70"/>
-      <c r="AR14" s="70"/>
-      <c r="AS14" s="70"/>
-      <c r="AT14" s="70"/>
-      <c r="AU14" s="70"/>
-      <c r="AV14" s="70"/>
-      <c r="AW14" s="70"/>
-      <c r="AX14" s="70"/>
-      <c r="AY14" s="70"/>
-      <c r="AZ14" s="70"/>
-      <c r="BA14" s="70"/>
-      <c r="BB14" s="70"/>
-      <c r="BC14" s="70"/>
-      <c r="BD14" s="70"/>
-      <c r="BE14" s="70"/>
-      <c r="BF14" s="70"/>
-      <c r="BG14" s="70"/>
-      <c r="BH14" s="70"/>
-      <c r="BI14" s="70"/>
-      <c r="BJ14" s="70"/>
-      <c r="BK14" s="70"/>
-      <c r="BL14" s="70"/>
-      <c r="BM14" s="70"/>
-      <c r="BN14" s="70"/>
-      <c r="BO14" s="70"/>
-      <c r="BP14" s="71"/>
-      <c r="BQ14" s="109"/>
+      <c r="H14" s="134"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="52"/>
+      <c r="L14" s="52"/>
+      <c r="M14" s="52"/>
+      <c r="N14" s="52"/>
+      <c r="O14" s="52"/>
+      <c r="P14" s="52"/>
+      <c r="Q14" s="53"/>
+      <c r="R14" s="52"/>
+      <c r="S14" s="52"/>
+      <c r="T14" s="52"/>
+      <c r="U14" s="52"/>
+      <c r="V14" s="52"/>
+      <c r="W14" s="52"/>
+      <c r="X14" s="52"/>
+      <c r="Y14" s="45"/>
+      <c r="Z14" s="52"/>
+      <c r="AA14" s="52"/>
+      <c r="AB14" s="52"/>
+      <c r="AC14" s="52"/>
+      <c r="AD14" s="52"/>
+      <c r="AE14" s="52"/>
+      <c r="AF14" s="52"/>
+      <c r="AG14" s="52"/>
+      <c r="AH14" s="52"/>
+      <c r="AI14" s="52"/>
+      <c r="AJ14" s="52"/>
+      <c r="AK14" s="52"/>
+      <c r="AL14" s="52"/>
+      <c r="AM14" s="52"/>
+      <c r="AN14" s="52"/>
+      <c r="AO14" s="52"/>
+      <c r="AP14" s="52"/>
+      <c r="AQ14" s="52"/>
+      <c r="AR14" s="52"/>
+      <c r="AS14" s="52"/>
+      <c r="AT14" s="52"/>
+      <c r="AU14" s="52"/>
+      <c r="AV14" s="52"/>
+      <c r="AW14" s="52"/>
+      <c r="AX14" s="52"/>
+      <c r="AY14" s="52"/>
+      <c r="AZ14" s="52"/>
+      <c r="BA14" s="52"/>
+      <c r="BB14" s="52"/>
+      <c r="BC14" s="52"/>
+      <c r="BD14" s="52"/>
+      <c r="BE14" s="52"/>
+      <c r="BF14" s="52"/>
+      <c r="BG14" s="52"/>
+      <c r="BH14" s="52"/>
+      <c r="BI14" s="52"/>
+      <c r="BJ14" s="52"/>
+      <c r="BK14" s="52"/>
+      <c r="BL14" s="52"/>
+      <c r="BM14" s="52"/>
+      <c r="BN14" s="52"/>
+      <c r="BO14" s="52"/>
+      <c r="BP14" s="52"/>
+      <c r="BQ14" s="95"/>
     </row>
     <row r="15" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="26"/>
-      <c r="B15" s="130" t="s">
+      <c r="A15" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="100" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="57"/>
+      <c r="D15" s="58">
+        <f>(D16*DATEDIF(E16,F16,"D")+D17*DATEDIF(E17,F17,"D")+D18*DATEDIF(E18,F18,"D")+D19*DATEDIF(E19,F19,"D")+D20*DATEDIF(E20,F20,"D")+D21*DATEDIF(E21,F21,"D")+D22*DATEDIF(E22,F22,"D"))/(DATEDIF(E16,F16,"D")+DATEDIF(E17,F17,"D")+DATEDIF(E18,F18,"D")+DATEDIF(E19,F19,"D")+DATEDIF(E20,F20,"D")+DATEDIF(E21,F21,"D")+DATEDIF(E22,F22,"D"))</f>
+        <v>4.4050632911392405E-2</v>
+      </c>
+      <c r="E15" s="59"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="142">
+        <f ca="1">DATEDIF(E16,NOW(), "D")/DATEDIF(E16,BQ7,"d")</f>
+        <v>8.4745762711864403E-2</v>
+      </c>
+      <c r="H15" s="142"/>
+      <c r="I15" s="61"/>
+      <c r="J15" s="61"/>
+      <c r="K15" s="61"/>
+      <c r="L15" s="61"/>
+      <c r="M15" s="61"/>
+      <c r="N15" s="61"/>
+      <c r="O15" s="61"/>
+      <c r="P15" s="61"/>
+      <c r="Q15" s="61"/>
+      <c r="R15" s="61"/>
+      <c r="S15" s="61"/>
+      <c r="T15" s="61"/>
+      <c r="U15" s="61"/>
+      <c r="V15" s="61"/>
+      <c r="W15" s="61"/>
+      <c r="X15" s="61"/>
+      <c r="Y15" s="81"/>
+      <c r="Z15" s="61"/>
+      <c r="AA15" s="61"/>
+      <c r="AB15" s="61"/>
+      <c r="AC15" s="61"/>
+      <c r="AD15" s="61"/>
+      <c r="AE15" s="61"/>
+      <c r="AF15" s="61"/>
+      <c r="AG15" s="61"/>
+      <c r="AH15" s="61"/>
+      <c r="AI15" s="61"/>
+      <c r="AJ15" s="61"/>
+      <c r="AK15" s="61"/>
+      <c r="AL15" s="61"/>
+      <c r="AM15" s="61"/>
+      <c r="AN15" s="61"/>
+      <c r="AO15" s="61"/>
+      <c r="AP15" s="61"/>
+      <c r="AQ15" s="61"/>
+      <c r="AR15" s="61"/>
+      <c r="AS15" s="61"/>
+      <c r="AT15" s="61"/>
+      <c r="AU15" s="61"/>
+      <c r="AV15" s="61"/>
+      <c r="AW15" s="61"/>
+      <c r="AX15" s="61"/>
+      <c r="AY15" s="61"/>
+      <c r="AZ15" s="61"/>
+      <c r="BA15" s="61"/>
+      <c r="BB15" s="61"/>
+      <c r="BC15" s="61"/>
+      <c r="BD15" s="61"/>
+      <c r="BE15" s="61"/>
+      <c r="BF15" s="61"/>
+      <c r="BG15" s="61"/>
+      <c r="BH15" s="61"/>
+      <c r="BI15" s="61"/>
+      <c r="BJ15" s="61"/>
+      <c r="BK15" s="61"/>
+      <c r="BL15" s="61"/>
+      <c r="BM15" s="61"/>
+      <c r="BN15" s="61"/>
+      <c r="BO15" s="61"/>
+      <c r="BP15" s="62"/>
+      <c r="BQ15" s="96"/>
+    </row>
+    <row r="16" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="26"/>
+      <c r="B16" s="127" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="131"/>
-      <c r="D15" s="61">
+      <c r="C16" s="128"/>
+      <c r="D16" s="54">
         <v>1</v>
       </c>
-      <c r="E15" s="89">
+      <c r="E16" s="78">
         <v>43998</v>
       </c>
-      <c r="F15" s="89">
-        <f>E15+1</f>
+      <c r="F16" s="78">
+        <f>E16+1</f>
         <v>43999</v>
       </c>
-      <c r="G15" s="62">
-        <f t="shared" si="11"/>
+      <c r="G16" s="119">
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="H15" s="63"/>
-      <c r="I15" s="64"/>
-      <c r="J15" s="65"/>
-      <c r="K15" s="65"/>
-      <c r="L15" s="65"/>
-      <c r="M15" s="65"/>
-      <c r="N15" s="65"/>
-      <c r="O15" s="65"/>
-      <c r="P15" s="65"/>
-      <c r="Q15" s="65"/>
-      <c r="R15" s="65"/>
-      <c r="S15" s="65"/>
-      <c r="T15" s="65"/>
-      <c r="U15" s="65"/>
-      <c r="V15" s="65"/>
-      <c r="W15" s="65"/>
-      <c r="X15" s="65"/>
-      <c r="Y15" s="45"/>
-      <c r="Z15" s="65"/>
-      <c r="AA15" s="65"/>
-      <c r="AB15" s="65"/>
-      <c r="AC15" s="65"/>
-      <c r="AD15" s="65"/>
-      <c r="AE15" s="65"/>
-      <c r="AF15" s="65"/>
-      <c r="AG15" s="65"/>
-      <c r="AH15" s="65"/>
-      <c r="AI15" s="65"/>
-      <c r="AJ15" s="65"/>
-      <c r="AK15" s="65"/>
-      <c r="AL15" s="65"/>
-      <c r="AM15" s="65"/>
-      <c r="AN15" s="65"/>
-      <c r="AO15" s="65"/>
-      <c r="AP15" s="65"/>
-      <c r="AQ15" s="65"/>
-      <c r="AR15" s="65"/>
-      <c r="AS15" s="65"/>
-      <c r="AT15" s="65"/>
-      <c r="AU15" s="65"/>
-      <c r="AV15" s="65"/>
-      <c r="AW15" s="65"/>
-      <c r="AX15" s="65"/>
-      <c r="AY15" s="65"/>
-      <c r="AZ15" s="65"/>
-      <c r="BA15" s="65"/>
-      <c r="BB15" s="65"/>
-      <c r="BC15" s="65"/>
-      <c r="BD15" s="65"/>
-      <c r="BE15" s="65"/>
-      <c r="BF15" s="65"/>
-      <c r="BG15" s="65"/>
-      <c r="BH15" s="65"/>
-      <c r="BI15" s="65"/>
-      <c r="BJ15" s="65"/>
-      <c r="BK15" s="65"/>
-      <c r="BL15" s="65"/>
-      <c r="BM15" s="65"/>
-      <c r="BN15" s="65"/>
-      <c r="BO15" s="65"/>
-      <c r="BP15" s="65"/>
-      <c r="BQ15" s="108"/>
-    </row>
-    <row r="16" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="26"/>
-      <c r="B16" s="128" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="129"/>
-      <c r="D16" s="13">
-        <v>0.05</v>
-      </c>
-      <c r="E16" s="90">
-        <f>F13-12</f>
-        <v>44000</v>
-      </c>
-      <c r="F16" s="90">
-        <f>E16+31</f>
-        <v>44031</v>
-      </c>
-      <c r="G16" s="55">
-        <f t="shared" si="11"/>
-        <v>32</v>
-      </c>
-      <c r="H16" s="53"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="35"/>
-      <c r="N16" s="35"/>
-      <c r="O16" s="35"/>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="35"/>
-      <c r="R16" s="35"/>
-      <c r="S16" s="35"/>
-      <c r="T16" s="35"/>
-      <c r="U16" s="35"/>
-      <c r="V16" s="35"/>
-      <c r="W16" s="35"/>
-      <c r="X16" s="35"/>
+      <c r="H16" s="120"/>
+      <c r="I16" s="55"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="56"/>
+      <c r="L16" s="56"/>
+      <c r="M16" s="56"/>
+      <c r="N16" s="56"/>
+      <c r="O16" s="56"/>
+      <c r="P16" s="56"/>
+      <c r="Q16" s="56"/>
+      <c r="R16" s="56"/>
+      <c r="S16" s="56"/>
+      <c r="T16" s="56"/>
+      <c r="U16" s="56"/>
+      <c r="V16" s="56"/>
+      <c r="W16" s="56"/>
+      <c r="X16" s="56"/>
       <c r="Y16" s="45"/>
-      <c r="Z16" s="35"/>
-      <c r="AA16" s="35"/>
-      <c r="AB16" s="35"/>
-      <c r="AC16" s="35"/>
-      <c r="AD16" s="35"/>
-      <c r="AE16" s="35"/>
-      <c r="AF16" s="35"/>
-      <c r="AG16" s="35"/>
-      <c r="AH16" s="35"/>
-      <c r="AI16" s="35"/>
-      <c r="AJ16" s="35"/>
-      <c r="AK16" s="35"/>
-      <c r="AL16" s="35"/>
-      <c r="AM16" s="35"/>
-      <c r="AN16" s="35"/>
-      <c r="AO16" s="35"/>
-      <c r="AP16" s="35"/>
-      <c r="AQ16" s="35"/>
-      <c r="AR16" s="35"/>
-      <c r="AS16" s="35"/>
-      <c r="AT16" s="35"/>
-      <c r="AU16" s="35"/>
-      <c r="AV16" s="35"/>
-      <c r="AW16" s="35"/>
-      <c r="AX16" s="35"/>
-      <c r="AY16" s="35"/>
-      <c r="AZ16" s="35"/>
-      <c r="BA16" s="35"/>
-      <c r="BB16" s="35"/>
-      <c r="BC16" s="35"/>
-      <c r="BD16" s="35"/>
-      <c r="BE16" s="35"/>
-      <c r="BF16" s="35"/>
-      <c r="BG16" s="35"/>
-      <c r="BH16" s="35"/>
-      <c r="BI16" s="35"/>
-      <c r="BJ16" s="35"/>
-      <c r="BK16" s="35"/>
-      <c r="BL16" s="35"/>
-      <c r="BM16" s="35"/>
-      <c r="BN16" s="35"/>
-      <c r="BO16" s="35"/>
-      <c r="BP16" s="35"/>
-      <c r="BQ16" s="108"/>
+      <c r="Z16" s="56"/>
+      <c r="AA16" s="56"/>
+      <c r="AB16" s="56"/>
+      <c r="AC16" s="56"/>
+      <c r="AD16" s="56"/>
+      <c r="AE16" s="56"/>
+      <c r="AF16" s="56"/>
+      <c r="AG16" s="56"/>
+      <c r="AH16" s="56"/>
+      <c r="AI16" s="56"/>
+      <c r="AJ16" s="56"/>
+      <c r="AK16" s="56"/>
+      <c r="AL16" s="56"/>
+      <c r="AM16" s="56"/>
+      <c r="AN16" s="56"/>
+      <c r="AO16" s="56"/>
+      <c r="AP16" s="56"/>
+      <c r="AQ16" s="56"/>
+      <c r="AR16" s="56"/>
+      <c r="AS16" s="56"/>
+      <c r="AT16" s="56"/>
+      <c r="AU16" s="56"/>
+      <c r="AV16" s="56"/>
+      <c r="AW16" s="56"/>
+      <c r="AX16" s="56"/>
+      <c r="AY16" s="56"/>
+      <c r="AZ16" s="56"/>
+      <c r="BA16" s="56"/>
+      <c r="BB16" s="56"/>
+      <c r="BC16" s="56"/>
+      <c r="BD16" s="56"/>
+      <c r="BE16" s="56"/>
+      <c r="BF16" s="56"/>
+      <c r="BG16" s="56"/>
+      <c r="BH16" s="56"/>
+      <c r="BI16" s="56"/>
+      <c r="BJ16" s="56"/>
+      <c r="BK16" s="56"/>
+      <c r="BL16" s="56"/>
+      <c r="BM16" s="56"/>
+      <c r="BN16" s="56"/>
+      <c r="BO16" s="56"/>
+      <c r="BP16" s="56"/>
+      <c r="BQ16" s="95"/>
     </row>
     <row r="17" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="25"/>
-      <c r="B17" s="128" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="129"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="125" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="126"/>
       <c r="D17" s="13">
-        <v>0</v>
-      </c>
-      <c r="E17" s="90">
-        <f>F16-7</f>
-        <v>44024</v>
-      </c>
-      <c r="F17" s="90">
-        <f>E17+7</f>
+        <v>0.08</v>
+      </c>
+      <c r="E17" s="79">
+        <f>F14-12</f>
+        <v>44000</v>
+      </c>
+      <c r="F17" s="79">
+        <f>E17+31</f>
         <v>44031</v>
       </c>
-      <c r="G17" s="55">
-        <f t="shared" si="11"/>
-        <v>8</v>
-      </c>
-      <c r="H17" s="53"/>
+      <c r="G17" s="114">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="H17" s="115"/>
       <c r="I17" s="49"/>
       <c r="J17" s="35"/>
       <c r="K17" s="35"/>
@@ -4035,7 +4613,7 @@
       <c r="V17" s="35"/>
       <c r="W17" s="35"/>
       <c r="X17" s="35"/>
-      <c r="Y17" s="46"/>
+      <c r="Y17" s="45"/>
       <c r="Z17" s="35"/>
       <c r="AA17" s="35"/>
       <c r="AB17" s="35"/>
@@ -4079,30 +4657,30 @@
       <c r="BN17" s="35"/>
       <c r="BO17" s="35"/>
       <c r="BP17" s="35"/>
-      <c r="BQ17" s="108"/>
+      <c r="BQ17" s="95"/>
     </row>
     <row r="18" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="25"/>
-      <c r="B18" s="128" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="129"/>
+      <c r="B18" s="125" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="126"/>
       <c r="D18" s="13">
         <v>0</v>
       </c>
-      <c r="E18" s="90">
-        <f>F16-7</f>
+      <c r="E18" s="79">
+        <f>F17-7</f>
         <v>44024</v>
       </c>
-      <c r="F18" s="90">
-        <f>E18+10</f>
-        <v>44034</v>
-      </c>
-      <c r="G18" s="55">
-        <f t="shared" si="11"/>
-        <v>11</v>
-      </c>
-      <c r="H18" s="53"/>
+      <c r="F18" s="79">
+        <f>E18+7</f>
+        <v>44031</v>
+      </c>
+      <c r="G18" s="114">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="H18" s="115"/>
       <c r="I18" s="49"/>
       <c r="J18" s="35"/>
       <c r="K18" s="35"/>
@@ -4115,11 +4693,11 @@
       <c r="R18" s="35"/>
       <c r="S18" s="35"/>
       <c r="T18" s="35"/>
-      <c r="U18" s="36"/>
-      <c r="V18" s="36"/>
+      <c r="U18" s="35"/>
+      <c r="V18" s="35"/>
       <c r="W18" s="35"/>
       <c r="X18" s="35"/>
-      <c r="Y18" s="45"/>
+      <c r="Y18" s="46"/>
       <c r="Z18" s="35"/>
       <c r="AA18" s="35"/>
       <c r="AB18" s="35"/>
@@ -4163,30 +4741,30 @@
       <c r="BN18" s="35"/>
       <c r="BO18" s="35"/>
       <c r="BP18" s="35"/>
-      <c r="BQ18" s="108"/>
+      <c r="BQ18" s="95"/>
     </row>
     <row r="19" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="25"/>
-      <c r="B19" s="128" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="129"/>
+      <c r="B19" s="125" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="126"/>
       <c r="D19" s="13">
         <v>0</v>
       </c>
-      <c r="E19" s="90">
-        <f>F18-3</f>
-        <v>44031</v>
-      </c>
-      <c r="F19" s="90">
+      <c r="E19" s="79">
+        <f>F17-7</f>
+        <v>44024</v>
+      </c>
+      <c r="F19" s="79">
         <f>E19+10</f>
-        <v>44041</v>
-      </c>
-      <c r="G19" s="55">
-        <f t="shared" si="11"/>
+        <v>44034</v>
+      </c>
+      <c r="G19" s="114">
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="H19" s="53"/>
+      <c r="H19" s="115"/>
       <c r="I19" s="49"/>
       <c r="J19" s="35"/>
       <c r="K19" s="35"/>
@@ -4199,8 +4777,8 @@
       <c r="R19" s="35"/>
       <c r="S19" s="35"/>
       <c r="T19" s="35"/>
-      <c r="U19" s="35"/>
-      <c r="V19" s="35"/>
+      <c r="U19" s="36"/>
+      <c r="V19" s="36"/>
       <c r="W19" s="35"/>
       <c r="X19" s="35"/>
       <c r="Y19" s="45"/>
@@ -4247,30 +4825,30 @@
       <c r="BN19" s="35"/>
       <c r="BO19" s="35"/>
       <c r="BP19" s="35"/>
-      <c r="BQ19" s="108"/>
+      <c r="BQ19" s="95"/>
     </row>
     <row r="20" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="25"/>
-      <c r="B20" s="128" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="129"/>
+      <c r="B20" s="125" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="126"/>
       <c r="D20" s="13">
         <v>0</v>
       </c>
-      <c r="E20" s="90">
-        <f>F18</f>
-        <v>44034</v>
-      </c>
-      <c r="F20" s="90">
-        <f>E20+9</f>
-        <v>44043</v>
-      </c>
-      <c r="G20" s="55">
-        <f t="shared" si="11"/>
-        <v>10</v>
-      </c>
-      <c r="H20" s="53"/>
+      <c r="E20" s="79">
+        <f>F19-3</f>
+        <v>44031</v>
+      </c>
+      <c r="F20" s="79">
+        <f>E20+10</f>
+        <v>44041</v>
+      </c>
+      <c r="G20" s="114">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="H20" s="115"/>
       <c r="I20" s="49"/>
       <c r="J20" s="35"/>
       <c r="K20" s="35"/>
@@ -4331,141 +4909,227 @@
       <c r="BN20" s="35"/>
       <c r="BO20" s="35"/>
       <c r="BP20" s="35"/>
-      <c r="BQ20" s="108"/>
+      <c r="BQ20" s="95"/>
     </row>
     <row r="21" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="25"/>
-      <c r="B21" s="126" t="s">
+      <c r="B21" s="125" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="126"/>
+      <c r="D21" s="13">
+        <v>0</v>
+      </c>
+      <c r="E21" s="79">
+        <f>F19</f>
+        <v>44034</v>
+      </c>
+      <c r="F21" s="79">
+        <f>E21+10</f>
+        <v>44044</v>
+      </c>
+      <c r="G21" s="114">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="H21" s="115"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="35"/>
+      <c r="M21" s="35"/>
+      <c r="N21" s="35"/>
+      <c r="O21" s="35"/>
+      <c r="P21" s="35"/>
+      <c r="Q21" s="35"/>
+      <c r="R21" s="35"/>
+      <c r="S21" s="35"/>
+      <c r="T21" s="35"/>
+      <c r="U21" s="35"/>
+      <c r="V21" s="35"/>
+      <c r="W21" s="35"/>
+      <c r="X21" s="35"/>
+      <c r="Y21" s="45"/>
+      <c r="Z21" s="35"/>
+      <c r="AA21" s="35"/>
+      <c r="AB21" s="35"/>
+      <c r="AC21" s="35"/>
+      <c r="AD21" s="35"/>
+      <c r="AE21" s="35"/>
+      <c r="AF21" s="35"/>
+      <c r="AG21" s="35"/>
+      <c r="AH21" s="35"/>
+      <c r="AI21" s="35"/>
+      <c r="AJ21" s="35"/>
+      <c r="AK21" s="35"/>
+      <c r="AL21" s="35"/>
+      <c r="AM21" s="35"/>
+      <c r="AN21" s="35"/>
+      <c r="AO21" s="35"/>
+      <c r="AP21" s="35"/>
+      <c r="AQ21" s="35"/>
+      <c r="AR21" s="35"/>
+      <c r="AS21" s="35"/>
+      <c r="AT21" s="35"/>
+      <c r="AU21" s="35"/>
+      <c r="AV21" s="35"/>
+      <c r="AW21" s="35"/>
+      <c r="AX21" s="35"/>
+      <c r="AY21" s="35"/>
+      <c r="AZ21" s="35"/>
+      <c r="BA21" s="35"/>
+      <c r="BB21" s="35"/>
+      <c r="BC21" s="35"/>
+      <c r="BD21" s="35"/>
+      <c r="BE21" s="35"/>
+      <c r="BF21" s="35"/>
+      <c r="BG21" s="35"/>
+      <c r="BH21" s="35"/>
+      <c r="BI21" s="35"/>
+      <c r="BJ21" s="35"/>
+      <c r="BK21" s="35"/>
+      <c r="BL21" s="35"/>
+      <c r="BM21" s="35"/>
+      <c r="BN21" s="35"/>
+      <c r="BO21" s="35"/>
+      <c r="BP21" s="35"/>
+      <c r="BQ21" s="95"/>
+    </row>
+    <row r="22" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="25"/>
+      <c r="B22" s="123" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="127"/>
-      <c r="D21" s="96">
+      <c r="C22" s="124"/>
+      <c r="D22" s="85">
         <v>0</v>
       </c>
-      <c r="E21" s="97">
-        <f>F20-5</f>
-        <v>44038</v>
-      </c>
-      <c r="F21" s="97">
-        <f>E21+12</f>
-        <v>44050</v>
-      </c>
-      <c r="G21" s="98">
-        <f t="shared" si="11"/>
-        <v>13</v>
-      </c>
-      <c r="H21" s="99"/>
-      <c r="I21" s="100"/>
-      <c r="J21" s="101"/>
-      <c r="K21" s="101"/>
-      <c r="L21" s="101"/>
-      <c r="M21" s="101"/>
-      <c r="N21" s="101"/>
-      <c r="O21" s="101"/>
-      <c r="P21" s="101"/>
-      <c r="Q21" s="101"/>
-      <c r="R21" s="101"/>
-      <c r="S21" s="101"/>
-      <c r="T21" s="101"/>
-      <c r="U21" s="101"/>
-      <c r="V21" s="101"/>
-      <c r="W21" s="101"/>
-      <c r="X21" s="101"/>
-      <c r="Y21" s="102"/>
-      <c r="Z21" s="101"/>
-      <c r="AA21" s="101"/>
-      <c r="AB21" s="101"/>
-      <c r="AC21" s="101"/>
-      <c r="AD21" s="101"/>
-      <c r="AE21" s="101"/>
-      <c r="AF21" s="101"/>
-      <c r="AG21" s="101"/>
-      <c r="AH21" s="101"/>
-      <c r="AI21" s="101"/>
-      <c r="AJ21" s="101"/>
-      <c r="AK21" s="101"/>
-      <c r="AL21" s="101"/>
-      <c r="AM21" s="101"/>
-      <c r="AN21" s="101"/>
-      <c r="AO21" s="101"/>
-      <c r="AP21" s="101"/>
-      <c r="AQ21" s="101"/>
-      <c r="AR21" s="101"/>
-      <c r="AS21" s="101"/>
-      <c r="AT21" s="101"/>
-      <c r="AU21" s="101"/>
-      <c r="AV21" s="101"/>
-      <c r="AW21" s="101"/>
-      <c r="AX21" s="101"/>
-      <c r="AY21" s="101"/>
-      <c r="AZ21" s="101"/>
-      <c r="BA21" s="101"/>
-      <c r="BB21" s="101"/>
-      <c r="BC21" s="101"/>
-      <c r="BD21" s="101"/>
-      <c r="BE21" s="101"/>
-      <c r="BF21" s="101"/>
-      <c r="BG21" s="101"/>
-      <c r="BH21" s="101"/>
-      <c r="BI21" s="101"/>
-      <c r="BJ21" s="101"/>
-      <c r="BK21" s="101"/>
-      <c r="BL21" s="101"/>
-      <c r="BM21" s="101"/>
-      <c r="BN21" s="101"/>
-      <c r="BO21" s="101"/>
-      <c r="BP21" s="101"/>
-      <c r="BQ21" s="110"/>
+      <c r="E22" s="86">
+        <f>F21-7</f>
+        <v>44037</v>
+      </c>
+      <c r="F22" s="86">
+        <f>E22+10</f>
+        <v>44047</v>
+      </c>
+      <c r="G22" s="116">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="H22" s="117"/>
+      <c r="I22" s="87"/>
+      <c r="J22" s="88"/>
+      <c r="K22" s="88"/>
+      <c r="L22" s="88"/>
+      <c r="M22" s="88"/>
+      <c r="N22" s="88"/>
+      <c r="O22" s="88"/>
+      <c r="P22" s="88"/>
+      <c r="Q22" s="88"/>
+      <c r="R22" s="88"/>
+      <c r="S22" s="88"/>
+      <c r="T22" s="88"/>
+      <c r="U22" s="88"/>
+      <c r="V22" s="88"/>
+      <c r="W22" s="88"/>
+      <c r="X22" s="88"/>
+      <c r="Y22" s="89"/>
+      <c r="Z22" s="88"/>
+      <c r="AA22" s="88"/>
+      <c r="AB22" s="88"/>
+      <c r="AC22" s="88"/>
+      <c r="AD22" s="88"/>
+      <c r="AE22" s="88"/>
+      <c r="AF22" s="88"/>
+      <c r="AG22" s="88"/>
+      <c r="AH22" s="88"/>
+      <c r="AI22" s="88"/>
+      <c r="AJ22" s="88"/>
+      <c r="AK22" s="88"/>
+      <c r="AL22" s="88"/>
+      <c r="AM22" s="88"/>
+      <c r="AN22" s="88"/>
+      <c r="AO22" s="88"/>
+      <c r="AP22" s="88"/>
+      <c r="AQ22" s="88"/>
+      <c r="AR22" s="88"/>
+      <c r="AS22" s="88"/>
+      <c r="AT22" s="88"/>
+      <c r="AU22" s="88"/>
+      <c r="AV22" s="88"/>
+      <c r="AW22" s="88"/>
+      <c r="AX22" s="88"/>
+      <c r="AY22" s="88"/>
+      <c r="AZ22" s="88"/>
+      <c r="BA22" s="88"/>
+      <c r="BB22" s="88"/>
+      <c r="BC22" s="88"/>
+      <c r="BD22" s="88"/>
+      <c r="BE22" s="88"/>
+      <c r="BF22" s="88"/>
+      <c r="BG22" s="88"/>
+      <c r="BH22" s="88"/>
+      <c r="BI22" s="88"/>
+      <c r="BJ22" s="88"/>
+      <c r="BK22" s="88"/>
+      <c r="BL22" s="88"/>
+      <c r="BM22" s="88"/>
+      <c r="BN22" s="88"/>
+      <c r="BO22" s="88"/>
+      <c r="BP22" s="88"/>
+      <c r="BQ22" s="97"/>
     </row>
-    <row r="22" spans="1:69" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="G22" s="6"/>
-    </row>
-    <row r="23" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="10"/>
-      <c r="F23" s="27"/>
+    <row r="23" spans="1:69" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="G23" s="6"/>
     </row>
     <row r="24" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="11"/>
+      <c r="C24" s="10"/>
+      <c r="F24" s="27"/>
+    </row>
+    <row r="25" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B19:C19"/>
+  <mergeCells count="36">
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B14:C14"/>
     <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="AR6:AX6"/>
+    <mergeCell ref="AY6:BE6"/>
+    <mergeCell ref="BF6:BL6"/>
+    <mergeCell ref="B7:G7"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="AR5:AX5"/>
-    <mergeCell ref="AY5:BE5"/>
-    <mergeCell ref="BF5:BL5"/>
-    <mergeCell ref="BM5:BQ5"/>
-    <mergeCell ref="G4:H5"/>
-    <mergeCell ref="I5:O5"/>
-    <mergeCell ref="P5:V5"/>
-    <mergeCell ref="W5:AC5"/>
-    <mergeCell ref="AD5:AJ5"/>
-    <mergeCell ref="AK5:AQ5"/>
-    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="BM6:BQ6"/>
+    <mergeCell ref="G5:H6"/>
+    <mergeCell ref="I6:O6"/>
+    <mergeCell ref="P6:V6"/>
+    <mergeCell ref="W6:AC6"/>
+    <mergeCell ref="AD6:AJ6"/>
+    <mergeCell ref="AK6:AQ6"/>
   </mergeCells>
-  <conditionalFormatting sqref="AF9:AF10 BH9:BH10 D8:D14 D16:D21">
-    <cfRule type="dataBar" priority="38">
+  <conditionalFormatting sqref="AF10:AF11 BH10:BH11 D9:D15 D17:D22">
+    <cfRule type="dataBar" priority="40">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4478,21 +5142,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I10:BP13 I21:BL21 BM20:BP21 I16:BP20 BQ6:BQ7 I6:BP8">
-    <cfRule type="expression" dxfId="14" priority="57">
-      <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
+  <conditionalFormatting sqref="I11:BP14 I22:BL22 BM21:BP22 I17:BP21 BQ7:BQ8 I7:BP9">
+    <cfRule type="expression" dxfId="29" priority="59">
+      <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I8:BP8 I10:BP13 I21:BL21 BM20:BP21 I16:BP20">
-    <cfRule type="expression" dxfId="13" priority="51">
-      <formula>AND(task_start&lt;=I$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$6)</formula>
+  <conditionalFormatting sqref="I9:BP9 I11:BP14 I22:BL22 BM21:BP22 I17:BP21">
+    <cfRule type="expression" dxfId="28" priority="53">
+      <formula>AND(task_start&lt;=I$7,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$7)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="52" stopIfTrue="1">
-      <formula>AND(task_end&gt;=I$6,task_start&lt;J$6)</formula>
+    <cfRule type="expression" dxfId="27" priority="54" stopIfTrue="1">
+      <formula>AND(task_end&gt;=I$7,task_start&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D20">
-    <cfRule type="dataBar" priority="18">
+  <conditionalFormatting sqref="D21">
+    <cfRule type="dataBar" priority="20">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4505,34 +5169,34 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20:BL20">
-    <cfRule type="expression" dxfId="11" priority="21">
-      <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
+  <conditionalFormatting sqref="I21:BL21">
+    <cfRule type="expression" dxfId="26" priority="23">
+      <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20:BL20">
-    <cfRule type="expression" dxfId="10" priority="19">
-      <formula>AND(task_start&lt;=I$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$6)</formula>
+  <conditionalFormatting sqref="I21:BL21">
+    <cfRule type="expression" dxfId="25" priority="21">
+      <formula>AND(task_start&lt;=I$7,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$7)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="20" stopIfTrue="1">
-      <formula>AND(task_end&gt;=I$6,task_start&lt;J$6)</formula>
+    <cfRule type="expression" dxfId="24" priority="22" stopIfTrue="1">
+      <formula>AND(task_end&gt;=I$7,task_start&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BQ8 BQ10:BQ13 BQ16:BQ21">
-    <cfRule type="expression" dxfId="8" priority="59">
-      <formula>AND(TODAY()&gt;=BQ$6,TODAY()&lt;#REF!)</formula>
+  <conditionalFormatting sqref="BQ9 BQ11:BQ14 BQ17:BQ22">
+    <cfRule type="expression" dxfId="23" priority="61">
+      <formula>AND(TODAY()&gt;=BQ$7,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BQ8 BQ10:BQ13 BQ16:BQ21">
-    <cfRule type="expression" dxfId="7" priority="62">
-      <formula>AND(task_start&lt;=BQ$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BQ$6)</formula>
+  <conditionalFormatting sqref="BQ9 BQ11:BQ14 BQ17:BQ22">
+    <cfRule type="expression" dxfId="22" priority="64">
+      <formula>AND(task_start&lt;=BQ$7,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BQ$7)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="63" stopIfTrue="1">
-      <formula>AND(task_end&gt;=BQ$6,task_start&lt;#REF!)</formula>
+    <cfRule type="expression" dxfId="21" priority="65" stopIfTrue="1">
+      <formula>AND(task_end&gt;=BQ$7,task_start&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15">
-    <cfRule type="dataBar" priority="1">
+  <conditionalFormatting sqref="D16">
+    <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4545,39 +5209,67 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I15:BP15">
-    <cfRule type="expression" dxfId="5" priority="4">
-      <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
+  <conditionalFormatting sqref="I16:BP16">
+    <cfRule type="expression" dxfId="20" priority="6">
+      <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BQ15">
-    <cfRule type="expression" dxfId="4" priority="5">
-      <formula>AND(TODAY()&gt;=BQ$6,TODAY()&lt;#REF!)</formula>
+  <conditionalFormatting sqref="BQ16">
+    <cfRule type="expression" dxfId="19" priority="7">
+      <formula>AND(TODAY()&gt;=BQ$7,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BQ15">
-    <cfRule type="expression" dxfId="3" priority="6">
-      <formula>AND(task_start&lt;=BQ$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BQ$6)</formula>
+  <conditionalFormatting sqref="BQ16">
+    <cfRule type="expression" dxfId="18" priority="8">
+      <formula>AND(task_start&lt;=BQ$7,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BQ$7)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="7" stopIfTrue="1">
-      <formula>AND(task_end&gt;=BQ$6,task_start&lt;#REF!)</formula>
+    <cfRule type="expression" dxfId="17" priority="9" stopIfTrue="1">
+      <formula>AND(task_end&gt;=BQ$7,task_start&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I15:BP15">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>AND(task_start&lt;=I$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$6)</formula>
+  <conditionalFormatting sqref="I16:BP16">
+    <cfRule type="expression" dxfId="16" priority="4">
+      <formula>AND(task_start&lt;=I$7,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$7)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
-      <formula>AND(task_end&gt;=I$6,task_start&lt;J$6)</formula>
+    <cfRule type="expression" dxfId="15" priority="5" stopIfTrue="1">
+      <formula>AND(task_end&gt;=I$7,task_start&lt;J$7)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G10:H10">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{963BBD81-685C-4709-8205-750E1428E766}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G15:H15">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{355DD565-805A-425C-AA09-35A2A15A797B}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Changing this number will scroll the Gantt Chart view." sqref="F5" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Changing this number will scroll the Gantt Chart view." sqref="F6" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>1</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="I3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="I4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="I2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
@@ -4602,7 +5294,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>AF9:AF10 BH9:BH10 D8:D14 D16:D21</xm:sqref>
+          <xm:sqref>AF10:AF11 BH10:BH11 D9:D15 D17:D22</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{B11F1B6D-5EC8-4017-96F0-3B2262CAA45A}">
@@ -4617,7 +5309,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D20</xm:sqref>
+          <xm:sqref>D21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{788803AA-61D0-401D-A7E2-8CCEAE2E2732}">
@@ -4632,7 +5324,37 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D15</xm:sqref>
+          <xm:sqref>D16</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{963BBD81-685C-4709-8205-750E1428E766}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G10:H10</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{355DD565-805A-425C-AA09-35A2A15A797B}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G15:H15</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>